<commit_message>
Harry - Export import for ui
</commit_message>
<xml_diff>
--- a/PythonProject/gui/Remote_Services.xlsx
+++ b/PythonProject/gui/Remote_Services.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="779" firstSheet="14" activeTab="21" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" tabRatio="779" firstSheet="6" activeTab="8" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demo Mode" sheetId="1" state="visible" r:id="rId1"/>
@@ -1453,7 +1453,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1528,7 +1528,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1669,7 +1669,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1744,7 +1744,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1885,7 +1885,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2027,7 +2027,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2269,7 +2269,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2421,7 +2421,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2573,7 +2573,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2725,7 +2725,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2954,7 +2954,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3106,7 +3106,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3335,7 +3335,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3487,7 +3487,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3639,7 +3639,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3781,7 +3781,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3847,7 +3847,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3967,7 +3967,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4196,7 +4196,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4271,7 +4271,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4413,7 +4413,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4490,7 +4490,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4600,7 +4600,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4752,7 +4752,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4904,7 +4904,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5056,7 +5056,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5208,7 +5208,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5360,7 +5360,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5512,7 +5512,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5664,7 +5664,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5739,7 +5739,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5891,7 +5891,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6582,7 +6582,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.1499069185460982"/>
+          <bgColor theme="0" tint="-0.1498764000366222"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10512,22 +10512,22 @@
       <selection activeCell="J16" sqref="I16:J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="3.28515625" customWidth="1" min="1" max="1"/>
-    <col width="6.85546875" customWidth="1" min="2" max="2"/>
-    <col width="16.28515625" customWidth="1" min="3" max="3"/>
-    <col width="14.42578125" customWidth="1" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
-    <col width="37.28515625" customWidth="1" min="6" max="6"/>
-    <col width="48.5703125" customWidth="1" min="7" max="7"/>
-    <col width="55.140625" customWidth="1" min="8" max="8"/>
-    <col width="39.42578125" customWidth="1" min="9" max="9"/>
+    <col width="3.26953125" customWidth="1" min="1" max="1"/>
+    <col width="6.81640625" customWidth="1" min="2" max="2"/>
+    <col width="16.26953125" customWidth="1" min="3" max="3"/>
+    <col width="14.453125" customWidth="1" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
+    <col width="37.26953125" customWidth="1" min="6" max="6"/>
+    <col width="48.54296875" customWidth="1" min="7" max="7"/>
+    <col width="55.1796875" customWidth="1" min="8" max="8"/>
+    <col width="39.453125" customWidth="1" min="9" max="9"/>
     <col width="47" customWidth="1" min="10" max="10"/>
-    <col width="14.5703125" customWidth="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="13.28515625" customWidth="1" min="14" max="14"/>
+    <col width="14.54296875" customWidth="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="13.26953125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -11433,24 +11433,24 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="56.42578125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="54.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="17.5703125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="2" min="17" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="56.453125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="54.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="17.54296875" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="2" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -12566,26 +12566,26 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="2.85546875" customWidth="1" min="1" max="1"/>
-    <col width="6.140625" customWidth="1" style="12" min="2" max="2"/>
+    <col width="2.81640625" customWidth="1" min="1" max="1"/>
+    <col width="6.1796875" customWidth="1" style="12" min="2" max="2"/>
     <col width="19" customWidth="1" style="12" min="3" max="3"/>
-    <col width="24.85546875" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
-    <col width="34.140625" customWidth="1" min="6" max="6"/>
-    <col width="46.140625" customWidth="1" min="7" max="7"/>
-    <col width="39.7109375" customWidth="1" min="8" max="8"/>
-    <col width="58.140625" customWidth="1" style="12" min="9" max="9"/>
-    <col width="61.28515625" customWidth="1" style="12" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="17.7109375" customWidth="1" min="14" max="14"/>
+    <col width="24.81640625" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
+    <col width="34.1796875" customWidth="1" min="6" max="6"/>
+    <col width="46.1796875" customWidth="1" min="7" max="7"/>
+    <col width="39.7265625" customWidth="1" min="8" max="8"/>
+    <col width="58.1796875" customWidth="1" style="12" min="9" max="9"/>
+    <col width="61.26953125" customWidth="1" style="12" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="12" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="17.7265625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -13494,26 +13494,26 @@
   </sheetPr>
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col width="3" customWidth="1" min="1" max="1"/>
-    <col width="7.140625" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
-    <col width="22.42578125" customWidth="1" style="12" min="3" max="3"/>
-    <col width="9.85546875" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
-    <col width="52.140625" customWidth="1" min="6" max="6"/>
-    <col width="41.85546875" customWidth="1" min="7" max="7"/>
-    <col width="45.85546875" customWidth="1" min="8" max="8"/>
-    <col width="53.140625" customWidth="1" style="12" min="9" max="9"/>
-    <col width="47.140625" customWidth="1" style="12" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="15.42578125" customWidth="1" min="14" max="14"/>
+    <col width="7.1796875" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
+    <col width="22.453125" customWidth="1" style="12" min="3" max="3"/>
+    <col width="9.81640625" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
+    <col width="52.1796875" customWidth="1" min="6" max="6"/>
+    <col width="41.81640625" customWidth="1" min="7" max="7"/>
+    <col width="45.81640625" customWidth="1" min="8" max="8"/>
+    <col width="53.1796875" customWidth="1" style="12" min="9" max="9"/>
+    <col width="47.1796875" customWidth="1" style="12" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="12" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="15.453125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -15346,28 +15346,28 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="2.42578125" customWidth="1" style="2" min="1" max="1"/>
-    <col width="6.140625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="21.85546875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="18.42578125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="68.140625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="43.7109375" customWidth="1" style="2" min="7" max="7"/>
-    <col width="50.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.85546875" customWidth="1" style="1" min="9" max="9"/>
-    <col width="53.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="2" min="17" max="16384"/>
+    <col width="2.453125" customWidth="1" style="2" min="1" max="1"/>
+    <col width="6.1796875" customWidth="1" style="2" min="2" max="2"/>
+    <col width="21.81640625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="18.453125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="68.1796875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="43.7265625" customWidth="1" style="2" min="7" max="7"/>
+    <col width="50.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.81640625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="53.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="16.81640625" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="2" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -16322,28 +16322,28 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="60.140625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="48.85546875" customWidth="1" style="2" min="7" max="7"/>
-    <col width="60.140625" customWidth="1" style="2" min="8" max="8"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="60.1796875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="48.81640625" customWidth="1" style="2" min="7" max="7"/>
+    <col width="60.1796875" customWidth="1" style="2" min="8" max="8"/>
     <col width="63" customWidth="1" style="1" min="9" max="9"/>
-    <col width="49.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="2" min="17" max="16384"/>
+    <col width="49.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.81640625" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="2" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -17189,20 +17189,20 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="2.85546875" customWidth="1" min="1" max="1"/>
+    <col width="2.81640625" customWidth="1" min="1" max="1"/>
     <col width="26" customWidth="1" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
-    <col width="42.85546875" customWidth="1" min="6" max="6"/>
-    <col width="47.5703125" customWidth="1" min="7" max="7"/>
-    <col width="38.85546875" customWidth="1" min="8" max="8"/>
-    <col width="37.42578125" customWidth="1" min="9" max="9"/>
-    <col width="50.85546875" customWidth="1" min="10" max="10"/>
-    <col width="17.5703125" customWidth="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="18.140625" customWidth="1" min="14" max="14"/>
+    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
+    <col width="42.81640625" customWidth="1" min="6" max="6"/>
+    <col width="47.54296875" customWidth="1" min="7" max="7"/>
+    <col width="38.81640625" customWidth="1" min="8" max="8"/>
+    <col width="37.453125" customWidth="1" min="9" max="9"/>
+    <col width="50.81640625" customWidth="1" min="10" max="10"/>
+    <col width="17.54296875" customWidth="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="18.1796875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -17801,24 +17801,24 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="56.42578125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="45.7109375" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="20.42578125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="2" min="17" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="56.453125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="45.7265625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="20.453125" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="2" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -18233,28 +18233,28 @@
   </sheetPr>
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView topLeftCell="C5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="43" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="80" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="43" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="43" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="43" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="44" min="9" max="9"/>
-    <col width="47.85546875" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
-    <col width="16.5703125" customWidth="1" style="43" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="43" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="43" min="17" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="43" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="80" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="43" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="43" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="43" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="44" min="9" max="9"/>
+    <col width="47.81640625" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
+    <col width="16.54296875" customWidth="1" style="43" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="43" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="43" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -18717,27 +18717,27 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="47.7109375" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.140625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="2" min="17" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="47.7265625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.1796875" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="2" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -19798,25 +19798,25 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="3.28515625" customWidth="1" min="1" max="1"/>
-    <col width="6.5703125" customWidth="1" min="2" max="2"/>
-    <col width="9.140625" customWidth="1" min="3" max="3"/>
-    <col width="13.28515625" customWidth="1" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
-    <col width="47.7109375" customWidth="1" min="6" max="6"/>
-    <col width="44.28515625" customWidth="1" min="7" max="7"/>
-    <col width="49.140625" customWidth="1" min="8" max="8"/>
-    <col width="47.140625" customWidth="1" min="9" max="10"/>
-    <col width="16.85546875" customWidth="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="15.85546875" customWidth="1" min="14" max="14"/>
+    <col width="3.26953125" customWidth="1" min="1" max="1"/>
+    <col width="6.54296875" customWidth="1" min="2" max="2"/>
+    <col width="9.1796875" customWidth="1" min="3" max="3"/>
+    <col width="13.26953125" customWidth="1" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
+    <col width="47.7265625" customWidth="1" min="6" max="6"/>
+    <col width="44.26953125" customWidth="1" min="7" max="7"/>
+    <col width="49.1796875" customWidth="1" min="8" max="8"/>
+    <col width="47.1796875" customWidth="1" min="9" max="10"/>
+    <col width="16.81640625" customWidth="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="15.81640625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -20511,28 +20511,28 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="D42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
+    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
     <col width="19" customWidth="1" style="80" min="3" max="3"/>
-    <col width="18.5703125" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
-    <col width="60.140625" customWidth="1" style="43" min="6" max="6"/>
-    <col width="48.85546875" customWidth="1" style="43" min="7" max="7"/>
-    <col width="78.28515625" customWidth="1" style="43" min="8" max="8"/>
-    <col width="52.28515625" customWidth="1" style="44" min="9" max="9"/>
-    <col width="43.5703125" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
-    <col width="18.7109375" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="46" min="17" max="16384"/>
+    <col width="18.54296875" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
+    <col width="60.1796875" customWidth="1" style="43" min="6" max="6"/>
+    <col width="48.81640625" customWidth="1" style="43" min="7" max="7"/>
+    <col width="78.26953125" customWidth="1" style="43" min="8" max="8"/>
+    <col width="52.26953125" customWidth="1" style="44" min="9" max="9"/>
+    <col width="43.54296875" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
+    <col width="18.7265625" customWidth="1" style="46" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="46" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="46" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -23334,21 +23334,21 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="42.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.42578125" customWidth="1" min="14" max="14"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="42.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.453125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -23711,21 +23711,21 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
     <col width="47" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.85546875" customWidth="1" min="14" max="14"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.81640625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -24018,24 +24018,24 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col width="2" customWidth="1" min="1" max="1"/>
-    <col width="16.140625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13.140625" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
+    <col width="16.1796875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.1796875" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
     <col width="44" customWidth="1" style="12" min="6" max="6"/>
-    <col width="51.85546875" customWidth="1" style="12" min="7" max="7"/>
-    <col width="41.5703125" customWidth="1" style="12" min="8" max="8"/>
+    <col width="51.81640625" customWidth="1" style="12" min="7" max="7"/>
+    <col width="41.54296875" customWidth="1" style="12" min="8" max="8"/>
     <col width="45" customWidth="1" style="12" min="9" max="9"/>
-    <col width="47.85546875" customWidth="1" style="12" min="10" max="10"/>
+    <col width="47.81640625" customWidth="1" style="12" min="10" max="10"/>
     <col width="14" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
     <col width="16" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
@@ -24697,28 +24697,28 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="57.7109375" customWidth="1" style="2" min="6" max="6"/>
-    <col width="54.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="60.140625" customWidth="1" style="2" min="8" max="8"/>
-    <col width="60.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="48.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.42578125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="2" min="17" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="57.7265625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="54.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="60.1796875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="60.453125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="48.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.453125" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="2" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -25616,25 +25616,25 @@
   </sheetPr>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="67.85546875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="67.81640625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
     <col width="46" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.140625" customWidth="1" min="14" max="14"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.1796875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -26203,25 +26203,25 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="40.7109375" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.28515625" customWidth="1" min="14" max="14"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="40.7265625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.26953125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -26926,26 +26926,26 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="3.28515625" customWidth="1" min="1" max="1"/>
-    <col width="6.85546875" customWidth="1" min="2" max="2"/>
-    <col width="20.5703125" customWidth="1" min="3" max="3"/>
-    <col width="13.42578125" customWidth="1" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
-    <col width="37.28515625" customWidth="1" min="6" max="6"/>
-    <col width="48.5703125" customWidth="1" min="7" max="7"/>
-    <col width="55.140625" customWidth="1" min="8" max="8"/>
-    <col width="36.7109375" customWidth="1" min="9" max="9"/>
-    <col width="50.28515625" customWidth="1" min="10" max="10"/>
-    <col width="14.5703125" customWidth="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="17.7109375" customWidth="1" min="14" max="14"/>
+    <col width="3.26953125" customWidth="1" min="1" max="1"/>
+    <col width="6.81640625" customWidth="1" min="2" max="2"/>
+    <col width="20.54296875" customWidth="1" min="3" max="3"/>
+    <col width="13.453125" customWidth="1" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
+    <col width="37.26953125" customWidth="1" min="6" max="6"/>
+    <col width="48.54296875" customWidth="1" min="7" max="7"/>
+    <col width="55.1796875" customWidth="1" min="8" max="8"/>
+    <col width="36.7265625" customWidth="1" min="9" max="9"/>
+    <col width="50.26953125" customWidth="1" min="10" max="10"/>
+    <col width="14.54296875" customWidth="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="17.7265625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -28136,24 +28136,24 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="80" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="43" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="43" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="43" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="44" min="9" max="9"/>
-    <col width="42.28515625" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
+    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="80" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="43" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="43" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="43" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="44" min="9" max="9"/>
+    <col width="42.26953125" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
     <col width="14" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="46" min="17" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="46" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="46" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -28445,25 +28445,25 @@
   </sheetPr>
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView topLeftCell="E8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="90.140625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="47.85546875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.28515625" customWidth="1" min="14" max="14"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="90.1796875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="47.81640625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.26953125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -29039,25 +29039,25 @@
   </sheetPr>
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView topLeftCell="D55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="D50" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="28.5703125" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="40.42578125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="60.85546875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="28.54296875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="40.453125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="60.81640625" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
     <col width="41" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.140625" customWidth="1" min="14" max="14"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.1796875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -32733,25 +32733,25 @@
   </sheetPr>
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F7" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="60.140625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="48.85546875" customWidth="1" style="2" min="7" max="7"/>
-    <col width="78.28515625" customWidth="1" style="2" min="8" max="8"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="60.1796875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="48.81640625" customWidth="1" style="2" min="7" max="7"/>
+    <col width="78.26953125" customWidth="1" style="2" min="8" max="8"/>
     <col width="57" customWidth="1" style="1" min="9" max="9"/>
     <col width="45" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.140625" customWidth="1" min="14" max="14"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.1796875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -33838,25 +33838,25 @@
   </sheetPr>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="11.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="15.5703125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="11.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="15.54296875" customWidth="1" style="36" min="5" max="5"/>
     <col width="86" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
     <col width="65" customWidth="1" style="2" min="8" max="8"/>
-    <col width="58.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="49.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="17.42578125" customWidth="1" min="14" max="14"/>
+    <col width="58.453125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="49.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="17.453125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -38104,28 +38104,28 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
+    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
     <col width="19" customWidth="1" style="80" min="3" max="3"/>
-    <col width="18.5703125" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
-    <col width="60.140625" customWidth="1" style="43" min="6" max="6"/>
-    <col width="48.85546875" customWidth="1" style="43" min="7" max="7"/>
-    <col width="85.5703125" customWidth="1" style="43" min="8" max="8"/>
+    <col width="18.54296875" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
+    <col width="60.1796875" customWidth="1" style="43" min="6" max="6"/>
+    <col width="48.81640625" customWidth="1" style="43" min="7" max="7"/>
+    <col width="85.54296875" customWidth="1" style="43" min="8" max="8"/>
     <col width="63" customWidth="1" style="44" min="9" max="9"/>
-    <col width="38.140625" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
-    <col width="15.5703125" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="46" min="17" max="16384"/>
+    <col width="38.1796875" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
+    <col width="15.54296875" customWidth="1" style="46" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="46" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="46" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -38792,25 +38792,25 @@
   </sheetPr>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="12" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="12" min="3" max="3"/>
-    <col width="15.42578125" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
-    <col width="52.7109375" customWidth="1" min="6" max="6"/>
-    <col width="51.140625" customWidth="1" min="7" max="7"/>
-    <col width="55.85546875" customWidth="1" min="8" max="8"/>
-    <col width="58.140625" customWidth="1" style="12" min="9" max="9"/>
-    <col width="45.140625" customWidth="1" style="12" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="17.85546875" customWidth="1" min="14" max="14"/>
+    <col width="10.26953125" customWidth="1" style="12" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="12" min="3" max="3"/>
+    <col width="15.453125" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
+    <col width="52.7265625" customWidth="1" min="6" max="6"/>
+    <col width="51.1796875" customWidth="1" min="7" max="7"/>
+    <col width="55.81640625" customWidth="1" min="8" max="8"/>
+    <col width="58.1796875" customWidth="1" style="12" min="9" max="9"/>
+    <col width="45.1796875" customWidth="1" style="12" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="12" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="17.81640625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -39384,27 +39384,27 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="65" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="65" min="3" max="3"/>
-    <col width="15.42578125" customWidth="1" style="65" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="66" min="5" max="5"/>
-    <col width="52.7109375" customWidth="1" style="46" min="6" max="6"/>
-    <col width="51.140625" customWidth="1" style="46" min="7" max="7"/>
-    <col width="55.85546875" customWidth="1" style="46" min="8" max="8"/>
-    <col width="58.140625" customWidth="1" style="65" min="9" max="9"/>
-    <col width="43.42578125" customWidth="1" style="65" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="65" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="46" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="46" min="13" max="13"/>
-    <col width="14.85546875" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="46" min="17" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="65" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="65" min="3" max="3"/>
+    <col width="15.453125" customWidth="1" style="65" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="66" min="5" max="5"/>
+    <col width="52.7265625" customWidth="1" style="46" min="6" max="6"/>
+    <col width="51.1796875" customWidth="1" style="46" min="7" max="7"/>
+    <col width="55.81640625" customWidth="1" style="46" min="8" max="8"/>
+    <col width="58.1796875" customWidth="1" style="65" min="9" max="9"/>
+    <col width="43.453125" customWidth="1" style="65" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="65" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="46" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="46" min="13" max="13"/>
+    <col width="14.81640625" customWidth="1" style="46" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="46" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="46" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -39535,7 +39535,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="89.45" customHeight="1">
+    <row r="5" ht="89.5" customHeight="1">
       <c r="A5" s="43" t="n"/>
       <c r="B5" s="127" t="n">
         <v>1</v>
@@ -40134,24 +40134,24 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="25.42578125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="61.42578125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="47.85546875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="2" min="17" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="25.453125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="61.453125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="47.81640625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.81640625" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="2" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -40959,28 +40959,28 @@
   </sheetPr>
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="9.140625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="9.1796875" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
     <col width="24" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="69.85546875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="36.85546875" customWidth="1" style="2" min="7" max="7"/>
-    <col width="61.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="66.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="48.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="11.140625" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="14.7109375" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="2" min="17" max="16384"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="69.81640625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="36.81640625" customWidth="1" style="2" min="7" max="7"/>
+    <col width="61.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="66.453125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="48.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="11.1796875" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="14.7265625" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="2" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -42845,28 +42845,28 @@
   </sheetPr>
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="9.140625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="17.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="65.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="40.28515625" customWidth="1" style="2" min="7" max="7"/>
-    <col width="53.85546875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="66.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="46.28515625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="11.28515625" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="14.140625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="16"/>
-    <col width="8.7109375" customWidth="1" style="2" min="17" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="9.1796875" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="17.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="65.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="40.26953125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="53.81640625" customWidth="1" style="2" min="8" max="8"/>
+    <col width="66.453125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="46.26953125" customWidth="1" style="1" min="10" max="10"/>
+    <col width="11.26953125" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="14.1796875" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="18"/>
+    <col width="8.7265625" customWidth="1" style="2" min="19" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -43059,7 +43059,8 @@
       <c r="H6" s="53" t="inlineStr">
         <is>
           <t>• All Doors are closed
-• Vehicle is locked</t>
+• Vehicle is locked
+Ignition is Off</t>
         </is>
       </c>
       <c r="I6" s="53" t="inlineStr">
@@ -43111,7 +43112,8 @@
       <c r="H7" s="53" t="inlineStr">
         <is>
           <t>• All Doors are closed
-• Vehicle is unlocked</t>
+• Vehicle is unlocked
+Ignition is Off</t>
         </is>
       </c>
       <c r="I7" s="53" t="inlineStr">

</xml_diff>

<commit_message>
Updates before showing china
</commit_message>
<xml_diff>
--- a/PythonProject/gui/Remote_Services.xlsx
+++ b/PythonProject/gui/Remote_Services.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="779" firstSheet="19" activeTab="29" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-105" yWindow="0" windowWidth="22500" windowHeight="15585" tabRatio="779" firstSheet="14" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demo Mode" sheetId="1" state="visible" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <definedName name="OCat">#REF!</definedName>
     <definedName name="Passed">[1]Dashboard!$E$17:INDEX([1]Dashboard!$E$17:$E$49,COUNT([1]Dashboard!$E$17:$E$49,"&lt;=0"))</definedName>
     <definedName name="Priority">[1]ChartBox!#REF!</definedName>
-    <definedName name="Service">OFFSET([2]Dashboard!$C$15,0,0,COUNTA([2]Dashboard!$C$15:$C$100)-1,1)</definedName>
+    <definedName name="Service">OFFSET([3]Dashboard!$C$15,0,0,COUNTA([3]Dashboard!$C$15:$C$100)-1,1)</definedName>
     <definedName name="Service_Name">[1]Dashboard!$C$17:INDEX([1]Dashboard!$C$17:$C$49,COUNTIF([1]Dashboard!$C$17:$C$49,"?*"))</definedName>
     <definedName name="Status">[1]ChartBox!#REF!</definedName>
     <definedName name="TCIncomplete">[1]Dashboard!$J$17:INDEX([1]Dashboard!$J$17:$J$49,COUNTIF([1]Dashboard!$J$17:$J$49,"?*"))</definedName>
@@ -73,14 +73,14 @@
     <definedName name="Failed" localSheetId="29">OFFSET(#REF!,0,0,COUNTA(#REF!)-1,1)</definedName>
     <definedName name="NA" localSheetId="29">OFFSET(#REF!,0,0,COUNTA(#REF!)-1,1)</definedName>
     <definedName name="Passed" localSheetId="29">OFFSET(#REF!,0,0,COUNTA(#REF!)-1,1)</definedName>
-    <definedName name="Priority" localSheetId="29">[3]ChartBox!#REF!</definedName>
+    <definedName name="Priority" localSheetId="29">[2]ChartBox!#REF!</definedName>
     <definedName name="Service" localSheetId="29">OFFSET(#REF!,0,0,COUNTA(#REF!)-1,1)</definedName>
-    <definedName name="Service_Name" localSheetId="29">[3]Dashboard!$C$17:INDEX([3]Dashboard!$C$17:$C$49,COUNTIF([3]Dashboard!$C$17:$C$49,"?*"))</definedName>
-    <definedName name="Status" localSheetId="29">[3]ChartBox!#REF!</definedName>
-    <definedName name="TCIncomplete" localSheetId="29">[3]Dashboard!$J$17:INDEX([3]Dashboard!$J$17:$J$49,COUNTIF([3]Dashboard!$J$17:$J$49,"?*"))</definedName>
-    <definedName name="TComplete" localSheetId="29">[3]Dashboard!$I$17:INDEX([3]Dashboard!$I$17:$I$49,COUNTIF([3]Dashboard!$I$17:$I$49,"?*"))</definedName>
-    <definedName name="TestType" localSheetId="29">[3]ChartBox!#REF!</definedName>
-    <definedName name="TIPercentage" localSheetId="29">(1-(SUM([3]Dashboard!$E$17:$E$49,[3]Dashboard!$F$17:$F$49, [3]Dashboard!$G$17:$G$49, [3]Dashboard!$H$17:$H$49))/SUM([3]Dashboard!$D$17:$D$49))*100</definedName>
+    <definedName name="Service_Name" localSheetId="29">[2]Dashboard!$C$17:INDEX([2]Dashboard!$C$17:$C$49,COUNTIF([2]Dashboard!$C$17:$C$49,"?*"))</definedName>
+    <definedName name="Status" localSheetId="29">[2]ChartBox!#REF!</definedName>
+    <definedName name="TCIncomplete" localSheetId="29">[2]Dashboard!$J$17:INDEX([2]Dashboard!$J$17:$J$49,COUNTIF([2]Dashboard!$J$17:$J$49,"?*"))</definedName>
+    <definedName name="TComplete" localSheetId="29">[2]Dashboard!$I$17:INDEX([2]Dashboard!$I$17:$I$49,COUNTIF([2]Dashboard!$I$17:$I$49,"?*"))</definedName>
+    <definedName name="TestType" localSheetId="29">[2]ChartBox!#REF!</definedName>
+    <definedName name="TIPercentage" localSheetId="29">(1-(SUM([2]Dashboard!$E$17:$E$49,[2]Dashboard!$F$17:$F$49, [2]Dashboard!$G$17:$G$49, [2]Dashboard!$H$17:$H$49))/SUM([2]Dashboard!$D$17:$D$49))*100</definedName>
   </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
@@ -9363,211 +9363,6 @@
       <sheetName val="ChartBox"/>
       <sheetName val="Change_History"/>
       <sheetName val="DemoMode"/>
-      <sheetName val="Customer_Enrollment"/>
-      <sheetName val="App_Registration_Pages-IDK"/>
-      <sheetName val="Add_VIN"/>
-      <sheetName val="MyBentleyAppLogin"/>
-      <sheetName val="Nickname"/>
-      <sheetName val="License(App)"/>
-      <sheetName val="VehicleStatusReport"/>
-      <sheetName val="RemoteLockUnlock"/>
-      <sheetName val="SingleServiceActivation"/>
-      <sheetName val="PHEV-MyCarStatistics"/>
-      <sheetName val="PHEV-MyCabinComfort"/>
-      <sheetName val="PHEV-MyBatteryCharge"/>
-      <sheetName val="RoadsideAssistanceCall(App)"/>
-      <sheetName val="DataServices"/>
-      <sheetName val="TheftAlarm"/>
-      <sheetName val="Audials(App)"/>
-      <sheetName val="CarFinder"/>
-      <sheetName val="NavCompanion"/>
-      <sheetName val="Notifications"/>
-      <sheetName val="PushNotifications"/>
-      <sheetName val="Profiles"/>
-      <sheetName val="TextStrings"/>
-      <sheetName val="PrivacyMode(App)"/>
-      <sheetName val="RemoteParkAssist"/>
-      <sheetName val="VehicleTrackingSystem"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="15">
-          <cell r="C15" t="str">
-            <v>DemoMode</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16" t="str">
-            <v>Customer_Enrollment</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17" t="str">
-            <v>App_Registration_Pages-IDK</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18" t="str">
-            <v>Add_VIN</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="C19" t="str">
-            <v>MyBentleyAppLogin</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="C20" t="str">
-            <v>Nickname</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="C21" t="str">
-            <v>License(App)</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="C22" t="str">
-            <v>VehicleStatusReport</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="C23" t="str">
-            <v>RemoteLockUnlock</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="C24" t="str">
-            <v>SingleServiceActivation</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="C25" t="str">
-            <v>PHEV-MyCarStatistics</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="C26" t="str">
-            <v>PHEV-MyCabinComfort</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="C27" t="str">
-            <v>PHEV-MyBatteryCharge</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="C28" t="str">
-            <v>RoadsideAssistanceCall(App)</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29" t="str">
-            <v>DataServices</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="C30" t="str">
-            <v>TheftAlarm</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31" t="str">
-            <v>Audials(App)</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="C32" t="str">
-            <v>CarFinder</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="C33" t="str">
-            <v>NavCompanion</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="C34" t="str">
-            <v>Notifications</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="C35" t="str">
-            <v>PushNotifications</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="C36" t="str">
-            <v>Profiles</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="C37" t="str">
-            <v>TextStrings</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="C38" t="str">
-            <v>PrivacyMode(App)</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="C39" t="str">
-            <v>RemoteParkAssist</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="C40" t="str">
-            <v>VehicleTrackingSystem</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="C41" t="str">
-            <v>Total Count</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Dashboard"/>
-      <sheetName val="ChartBox"/>
-      <sheetName val="Change_History"/>
-      <sheetName val="DemoMode"/>
       <sheetName val="App_Registration_Pages-IDK"/>
       <sheetName val="Add_VIN"/>
       <sheetName val="MyBentleyAppLogin"/>
@@ -10431,6 +10226,211 @@
       <sheetData sheetId="30" refreshError="1"/>
       <sheetData sheetId="31" refreshError="1"/>
       <sheetData sheetId="32" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Dashboard"/>
+      <sheetName val="ChartBox"/>
+      <sheetName val="Change_History"/>
+      <sheetName val="DemoMode"/>
+      <sheetName val="Customer_Enrollment"/>
+      <sheetName val="App_Registration_Pages-IDK"/>
+      <sheetName val="Add_VIN"/>
+      <sheetName val="MyBentleyAppLogin"/>
+      <sheetName val="Nickname"/>
+      <sheetName val="License(App)"/>
+      <sheetName val="VehicleStatusReport"/>
+      <sheetName val="RemoteLockUnlock"/>
+      <sheetName val="SingleServiceActivation"/>
+      <sheetName val="PHEV-MyCarStatistics"/>
+      <sheetName val="PHEV-MyCabinComfort"/>
+      <sheetName val="PHEV-MyBatteryCharge"/>
+      <sheetName val="RoadsideAssistanceCall(App)"/>
+      <sheetName val="DataServices"/>
+      <sheetName val="TheftAlarm"/>
+      <sheetName val="Audials(App)"/>
+      <sheetName val="CarFinder"/>
+      <sheetName val="NavCompanion"/>
+      <sheetName val="Notifications"/>
+      <sheetName val="PushNotifications"/>
+      <sheetName val="Profiles"/>
+      <sheetName val="TextStrings"/>
+      <sheetName val="PrivacyMode(App)"/>
+      <sheetName val="RemoteParkAssist"/>
+      <sheetName val="VehicleTrackingSystem"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="15">
+          <cell r="C15" t="str">
+            <v>DemoMode</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="C16" t="str">
+            <v>Customer_Enrollment</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="C17" t="str">
+            <v>App_Registration_Pages-IDK</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="C18" t="str">
+            <v>Add_VIN</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="C19" t="str">
+            <v>MyBentleyAppLogin</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="C20" t="str">
+            <v>Nickname</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="C21" t="str">
+            <v>License(App)</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="C22" t="str">
+            <v>VehicleStatusReport</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>RemoteLockUnlock</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24" t="str">
+            <v>SingleServiceActivation</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25" t="str">
+            <v>PHEV-MyCarStatistics</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="C26" t="str">
+            <v>PHEV-MyCabinComfort</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="C27" t="str">
+            <v>PHEV-MyBatteryCharge</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="C28" t="str">
+            <v>RoadsideAssistanceCall(App)</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29" t="str">
+            <v>DataServices</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="C30" t="str">
+            <v>TheftAlarm</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31" t="str">
+            <v>Audials(App)</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="C32" t="str">
+            <v>CarFinder</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33" t="str">
+            <v>NavCompanion</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34" t="str">
+            <v>Notifications</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35" t="str">
+            <v>PushNotifications</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36" t="str">
+            <v>Profiles</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37" t="str">
+            <v>TextStrings</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="C38" t="str">
+            <v>PrivacyMode(App)</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="C39" t="str">
+            <v>RemoteParkAssist</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="C40" t="str">
+            <v>VehicleTrackingSystem</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="C41" t="str">
+            <v>Total Count</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10729,8 +10729,8 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -11670,8 +11670,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="17.5703125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="2" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="2" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -13729,8 +13729,8 @@
   </sheetPr>
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -15581,8 +15581,8 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
@@ -15601,8 +15601,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" min="13" max="13"/>
     <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="2" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="2" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -16097,7 +16097,7 @@
       </c>
       <c r="F11" s="53" t="inlineStr">
         <is>
-          <t>Setting timer from vehicle</t>
+          <t>Setting timer from vehicle (Set first of two timers always)</t>
         </is>
       </c>
       <c r="G11" s="53" t="inlineStr">
@@ -16577,8 +16577,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="2" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="2" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -17489,7 +17489,7 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView topLeftCell="E8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -18121,8 +18121,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="20.42578125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="2" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="2" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -18557,8 +18557,8 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="16.5703125" customWidth="1" style="43" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="43" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="43" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="43" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="43" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -19040,8 +19040,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="15.140625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="2" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="2" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -20832,8 +20832,8 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="18.7109375" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="46" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="46" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -25018,8 +25018,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="15.42578125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="2" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="2" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -28452,8 +28452,8 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="14" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="46" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="46" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -34111,7 +34111,7 @@
   </sheetPr>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
@@ -38397,8 +38397,8 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="15.5703125" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="46" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="46" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -39632,8 +39632,8 @@
     <col width="19.42578125" customWidth="1" style="46" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="46" min="13" max="13"/>
     <col width="14.85546875" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="46" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="46" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -40393,8 +40393,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="15.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="2" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="2" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -41222,8 +41222,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="14.7109375" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="2" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="2" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -43108,8 +43108,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="14.140625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="29"/>
-    <col width="8.7109375" customWidth="1" style="2" min="30" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="30"/>
+    <col width="8.7109375" customWidth="1" style="2" min="31" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>

</xml_diff>

<commit_message>
Manual check feature added
</commit_message>
<xml_diff>
--- a/PythonProject/gui/Remote_Services.xlsx
+++ b/PythonProject/gui/Remote_Services.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="779" firstSheet="19" activeTab="29" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="779" firstSheet="19" activeTab="22" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demo Mode" sheetId="1" state="visible" r:id="rId1"/>
@@ -10733,22 +10733,22 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="3.28515625" customWidth="1" min="1" max="1"/>
-    <col width="6.85546875" customWidth="1" min="2" max="2"/>
-    <col width="16.28515625" customWidth="1" min="3" max="3"/>
-    <col width="14.42578125" customWidth="1" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
-    <col width="37.28515625" customWidth="1" min="6" max="6"/>
-    <col width="48.5703125" customWidth="1" min="7" max="7"/>
-    <col width="55.140625" customWidth="1" min="8" max="8"/>
-    <col width="39.42578125" customWidth="1" min="9" max="9"/>
+    <col width="3.26953125" customWidth="1" min="1" max="1"/>
+    <col width="6.81640625" customWidth="1" min="2" max="2"/>
+    <col width="16.26953125" customWidth="1" min="3" max="3"/>
+    <col width="14.453125" customWidth="1" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
+    <col width="37.26953125" customWidth="1" min="6" max="6"/>
+    <col width="48.54296875" customWidth="1" min="7" max="7"/>
+    <col width="55.1796875" customWidth="1" min="8" max="8"/>
+    <col width="39.453125" customWidth="1" min="9" max="9"/>
     <col width="47" customWidth="1" min="10" max="10"/>
-    <col width="14.5703125" customWidth="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="13.28515625" customWidth="1" min="14" max="14"/>
+    <col width="14.54296875" customWidth="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="13.26953125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -11654,24 +11654,24 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="56.42578125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="54.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="17.5703125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="2" min="33" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="56.453125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="54.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="17.54296875" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -12801,22 +12801,22 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="2.85546875" customWidth="1" min="1" max="1"/>
-    <col width="6.140625" customWidth="1" style="12" min="2" max="2"/>
+    <col width="2.81640625" customWidth="1" min="1" max="1"/>
+    <col width="6.1796875" customWidth="1" style="12" min="2" max="2"/>
     <col width="19" customWidth="1" style="12" min="3" max="3"/>
-    <col width="24.85546875" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
-    <col width="34.140625" customWidth="1" min="6" max="6"/>
-    <col width="46.140625" customWidth="1" min="7" max="7"/>
-    <col width="39.7109375" customWidth="1" min="8" max="8"/>
-    <col width="58.140625" customWidth="1" style="12" min="9" max="9"/>
-    <col width="61.28515625" customWidth="1" style="12" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="17.7109375" customWidth="1" min="14" max="14"/>
+    <col width="24.81640625" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
+    <col width="34.1796875" customWidth="1" min="6" max="6"/>
+    <col width="46.1796875" customWidth="1" min="7" max="7"/>
+    <col width="39.7265625" customWidth="1" min="8" max="8"/>
+    <col width="58.1796875" customWidth="1" style="12" min="9" max="9"/>
+    <col width="61.26953125" customWidth="1" style="12" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="12" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="17.7265625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -13733,22 +13733,22 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col width="3" customWidth="1" min="1" max="1"/>
-    <col width="7.140625" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
-    <col width="22.42578125" customWidth="1" style="12" min="3" max="3"/>
-    <col width="9.85546875" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
-    <col width="52.140625" customWidth="1" min="6" max="6"/>
-    <col width="41.85546875" customWidth="1" min="7" max="7"/>
-    <col width="45.85546875" customWidth="1" min="8" max="8"/>
-    <col width="53.140625" customWidth="1" style="12" min="9" max="9"/>
-    <col width="47.140625" customWidth="1" style="12" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="15.42578125" customWidth="1" min="14" max="14"/>
+    <col width="7.1796875" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
+    <col width="22.453125" customWidth="1" style="12" min="3" max="3"/>
+    <col width="9.81640625" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
+    <col width="52.1796875" customWidth="1" min="6" max="6"/>
+    <col width="41.81640625" customWidth="1" min="7" max="7"/>
+    <col width="45.81640625" customWidth="1" min="8" max="8"/>
+    <col width="53.1796875" customWidth="1" style="12" min="9" max="9"/>
+    <col width="47.1796875" customWidth="1" style="12" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="12" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="15.453125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -15585,24 +15585,24 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="2.42578125" customWidth="1" style="2" min="1" max="1"/>
-    <col width="6.140625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="21.85546875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="18.42578125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="68.140625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="43.7109375" customWidth="1" style="2" min="7" max="7"/>
-    <col width="50.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.85546875" customWidth="1" style="1" min="9" max="9"/>
-    <col width="53.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="2" min="33" max="16384"/>
+    <col width="2.453125" customWidth="1" style="2" min="1" max="1"/>
+    <col width="6.1796875" customWidth="1" style="2" min="2" max="2"/>
+    <col width="21.81640625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="18.453125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="68.1796875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="43.7265625" customWidth="1" style="2" min="7" max="7"/>
+    <col width="50.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.81640625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="53.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="16.81640625" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -16561,24 +16561,24 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="60.140625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="48.85546875" customWidth="1" style="2" min="7" max="7"/>
-    <col width="60.140625" customWidth="1" style="2" min="8" max="8"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="60.1796875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="48.81640625" customWidth="1" style="2" min="7" max="7"/>
+    <col width="60.1796875" customWidth="1" style="2" min="8" max="8"/>
     <col width="63" customWidth="1" style="1" min="9" max="9"/>
-    <col width="49.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="2" min="33" max="16384"/>
+    <col width="49.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.81640625" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -17493,20 +17493,20 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="2.85546875" customWidth="1" min="1" max="1"/>
+    <col width="2.81640625" customWidth="1" min="1" max="1"/>
     <col width="26" customWidth="1" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
-    <col width="42.85546875" customWidth="1" min="6" max="6"/>
-    <col width="47.5703125" customWidth="1" min="7" max="7"/>
-    <col width="38.85546875" customWidth="1" min="8" max="8"/>
-    <col width="37.42578125" customWidth="1" min="9" max="9"/>
-    <col width="50.85546875" customWidth="1" min="10" max="10"/>
-    <col width="17.5703125" customWidth="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="18.140625" customWidth="1" min="14" max="14"/>
+    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
+    <col width="42.81640625" customWidth="1" min="6" max="6"/>
+    <col width="47.54296875" customWidth="1" min="7" max="7"/>
+    <col width="38.81640625" customWidth="1" min="8" max="8"/>
+    <col width="37.453125" customWidth="1" min="9" max="9"/>
+    <col width="50.81640625" customWidth="1" min="10" max="10"/>
+    <col width="17.54296875" customWidth="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="18.1796875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -18105,24 +18105,24 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="56.42578125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="45.7109375" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="20.42578125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="2" min="33" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="56.453125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="45.7265625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="20.453125" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -18541,24 +18541,24 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="43" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="80" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="43" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="43" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="43" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="44" min="9" max="9"/>
-    <col width="47.85546875" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
-    <col width="16.5703125" customWidth="1" style="43" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="43" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="43" min="33" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="43" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="80" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="43" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="43" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="43" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="44" min="9" max="9"/>
+    <col width="47.81640625" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
+    <col width="16.54296875" customWidth="1" style="43" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="43" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="43" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -19024,24 +19024,24 @@
       <selection activeCell="J5" sqref="B5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="47.7109375" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.140625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="2" min="33" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="47.7265625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.1796875" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -20106,21 +20106,21 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="3.28515625" customWidth="1" min="1" max="1"/>
-    <col width="6.5703125" customWidth="1" min="2" max="2"/>
-    <col width="9.140625" customWidth="1" min="3" max="3"/>
-    <col width="13.28515625" customWidth="1" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
-    <col width="47.7109375" customWidth="1" min="6" max="6"/>
-    <col width="44.28515625" customWidth="1" min="7" max="7"/>
-    <col width="49.140625" customWidth="1" min="8" max="8"/>
-    <col width="47.140625" customWidth="1" min="9" max="10"/>
-    <col width="16.85546875" customWidth="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="15.85546875" customWidth="1" min="14" max="14"/>
+    <col width="3.26953125" customWidth="1" min="1" max="1"/>
+    <col width="6.54296875" customWidth="1" min="2" max="2"/>
+    <col width="9.1796875" customWidth="1" min="3" max="3"/>
+    <col width="13.26953125" customWidth="1" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
+    <col width="47.7265625" customWidth="1" min="6" max="6"/>
+    <col width="44.26953125" customWidth="1" min="7" max="7"/>
+    <col width="49.1796875" customWidth="1" min="8" max="8"/>
+    <col width="47.1796875" customWidth="1" min="9" max="10"/>
+    <col width="16.81640625" customWidth="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="15.81640625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -20816,24 +20816,24 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
+    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
     <col width="19" customWidth="1" style="80" min="3" max="3"/>
-    <col width="18.5703125" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
-    <col width="60.140625" customWidth="1" style="43" min="6" max="6"/>
-    <col width="48.85546875" customWidth="1" style="43" min="7" max="7"/>
-    <col width="78.28515625" customWidth="1" style="43" min="8" max="8"/>
-    <col width="52.28515625" customWidth="1" style="44" min="9" max="9"/>
-    <col width="43.5703125" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
-    <col width="18.7109375" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="46" min="33" max="16384"/>
+    <col width="18.54296875" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
+    <col width="60.1796875" customWidth="1" style="43" min="6" max="6"/>
+    <col width="48.81640625" customWidth="1" style="43" min="7" max="7"/>
+    <col width="78.26953125" customWidth="1" style="43" min="8" max="8"/>
+    <col width="52.26953125" customWidth="1" style="44" min="9" max="9"/>
+    <col width="43.54296875" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
+    <col width="18.7265625" customWidth="1" style="46" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="46" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="46" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -23635,21 +23635,21 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="42.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.42578125" customWidth="1" min="14" max="14"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="42.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.453125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -24012,21 +24012,21 @@
       <selection activeCell="E16" sqref="D16:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
     <col width="47" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.85546875" customWidth="1" min="14" max="14"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.81640625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -24323,20 +24323,20 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col width="2" customWidth="1" min="1" max="1"/>
-    <col width="16.140625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13.140625" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
+    <col width="16.1796875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.1796875" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
     <col width="44" customWidth="1" style="12" min="6" max="6"/>
-    <col width="51.85546875" customWidth="1" style="12" min="7" max="7"/>
-    <col width="41.5703125" customWidth="1" style="12" min="8" max="8"/>
+    <col width="51.81640625" customWidth="1" style="12" min="7" max="7"/>
+    <col width="41.54296875" customWidth="1" style="12" min="8" max="8"/>
     <col width="45" customWidth="1" style="12" min="9" max="9"/>
-    <col width="47.85546875" customWidth="1" style="12" min="10" max="10"/>
+    <col width="47.81640625" customWidth="1" style="12" min="10" max="10"/>
     <col width="14" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
     <col width="16" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
@@ -24998,28 +24998,28 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="G14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="57.7109375" customWidth="1" style="2" min="6" max="6"/>
-    <col width="54.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="60.140625" customWidth="1" style="2" min="8" max="8"/>
-    <col width="60.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="48.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.42578125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="2" min="33" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="57.7265625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="54.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="60.1796875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="60.453125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="48.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.453125" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -25917,21 +25917,21 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="67.85546875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="67.81640625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
     <col width="46" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.140625" customWidth="1" min="14" max="14"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.1796875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -26507,21 +26507,21 @@
       <selection activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="40.7109375" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.28515625" customWidth="1" min="14" max="14"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="40.7265625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.26953125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -27230,22 +27230,22 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="3.28515625" customWidth="1" min="1" max="1"/>
-    <col width="6.85546875" customWidth="1" min="2" max="2"/>
-    <col width="20.5703125" customWidth="1" min="3" max="3"/>
-    <col width="13.42578125" customWidth="1" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
-    <col width="37.28515625" customWidth="1" min="6" max="6"/>
-    <col width="48.5703125" customWidth="1" min="7" max="7"/>
-    <col width="55.140625" customWidth="1" min="8" max="8"/>
-    <col width="36.7109375" customWidth="1" min="9" max="9"/>
-    <col width="50.28515625" customWidth="1" min="10" max="10"/>
-    <col width="14.5703125" customWidth="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="17.7109375" customWidth="1" min="14" max="14"/>
+    <col width="3.26953125" customWidth="1" min="1" max="1"/>
+    <col width="6.81640625" customWidth="1" min="2" max="2"/>
+    <col width="20.54296875" customWidth="1" min="3" max="3"/>
+    <col width="13.453125" customWidth="1" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
+    <col width="37.26953125" customWidth="1" min="6" max="6"/>
+    <col width="48.54296875" customWidth="1" min="7" max="7"/>
+    <col width="55.1796875" customWidth="1" min="8" max="8"/>
+    <col width="36.7265625" customWidth="1" min="9" max="9"/>
+    <col width="50.26953125" customWidth="1" min="10" max="10"/>
+    <col width="14.54296875" customWidth="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="17.7265625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -28436,24 +28436,24 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="80" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="43" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="43" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="43" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="44" min="9" max="9"/>
-    <col width="42.28515625" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
+    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="80" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="43" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="43" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="43" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="44" min="9" max="9"/>
+    <col width="42.26953125" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
     <col width="14" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="46" min="33" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="46" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="46" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -28749,21 +28749,21 @@
       <selection activeCell="F5" sqref="F5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="90.140625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="47.85546875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.28515625" customWidth="1" min="14" max="14"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="90.1796875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="47.81640625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.26953125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -29343,21 +29343,21 @@
       <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="28.5703125" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="40.42578125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="60.85546875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="28.54296875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="40.453125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="60.81640625" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
     <col width="41" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.140625" customWidth="1" min="14" max="14"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.1796875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -33037,21 +33037,21 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="60.140625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="48.85546875" customWidth="1" style="2" min="7" max="7"/>
-    <col width="78.28515625" customWidth="1" style="2" min="8" max="8"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="60.1796875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="48.81640625" customWidth="1" style="2" min="7" max="7"/>
+    <col width="78.26953125" customWidth="1" style="2" min="8" max="8"/>
     <col width="57" customWidth="1" style="1" min="9" max="9"/>
     <col width="45" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.140625" customWidth="1" min="14" max="14"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.1796875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -34111,25 +34111,25 @@
   </sheetPr>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="11.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="15.5703125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="11.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="15.54296875" customWidth="1" style="36" min="5" max="5"/>
     <col width="86" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
     <col width="65" customWidth="1" style="2" min="8" max="8"/>
-    <col width="58.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="49.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="17.42578125" customWidth="1" min="14" max="14"/>
+    <col width="58.453125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="49.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="17.453125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -38381,24 +38381,24 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
+    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
     <col width="19" customWidth="1" style="80" min="3" max="3"/>
-    <col width="18.5703125" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
-    <col width="60.140625" customWidth="1" style="43" min="6" max="6"/>
-    <col width="48.85546875" customWidth="1" style="43" min="7" max="7"/>
-    <col width="85.5703125" customWidth="1" style="43" min="8" max="8"/>
+    <col width="18.54296875" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
+    <col width="60.1796875" customWidth="1" style="43" min="6" max="6"/>
+    <col width="48.81640625" customWidth="1" style="43" min="7" max="7"/>
+    <col width="85.54296875" customWidth="1" style="43" min="8" max="8"/>
     <col width="63" customWidth="1" style="44" min="9" max="9"/>
-    <col width="38.140625" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
-    <col width="15.5703125" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="46" min="33" max="16384"/>
+    <col width="38.1796875" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
+    <col width="15.54296875" customWidth="1" style="46" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="46" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="46" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -39029,21 +39029,21 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="10.28515625" customWidth="1" style="12" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="12" min="3" max="3"/>
-    <col width="15.42578125" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
-    <col width="52.7109375" customWidth="1" min="6" max="6"/>
-    <col width="51.140625" customWidth="1" min="7" max="7"/>
-    <col width="55.85546875" customWidth="1" min="8" max="8"/>
-    <col width="58.140625" customWidth="1" style="12" min="9" max="9"/>
-    <col width="45.140625" customWidth="1" style="12" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" min="13" max="13"/>
-    <col width="17.85546875" customWidth="1" min="14" max="14"/>
+    <col width="10.26953125" customWidth="1" style="12" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="12" min="3" max="3"/>
+    <col width="15.453125" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
+    <col width="52.7265625" customWidth="1" min="6" max="6"/>
+    <col width="51.1796875" customWidth="1" min="7" max="7"/>
+    <col width="55.81640625" customWidth="1" min="8" max="8"/>
+    <col width="58.1796875" customWidth="1" style="12" min="9" max="9"/>
+    <col width="45.1796875" customWidth="1" style="12" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="12" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="17.81640625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -39616,24 +39616,24 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="65" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="65" min="3" max="3"/>
-    <col width="15.42578125" customWidth="1" style="65" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="66" min="5" max="5"/>
-    <col width="52.7109375" customWidth="1" style="46" min="6" max="6"/>
-    <col width="51.140625" customWidth="1" style="46" min="7" max="7"/>
-    <col width="55.85546875" customWidth="1" style="46" min="8" max="8"/>
-    <col width="58.140625" customWidth="1" style="65" min="9" max="9"/>
-    <col width="43.42578125" customWidth="1" style="65" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="65" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="46" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="46" min="13" max="13"/>
-    <col width="14.85546875" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="46" min="33" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="65" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="65" min="3" max="3"/>
+    <col width="15.453125" customWidth="1" style="65" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="66" min="5" max="5"/>
+    <col width="52.7265625" customWidth="1" style="46" min="6" max="6"/>
+    <col width="51.1796875" customWidth="1" style="46" min="7" max="7"/>
+    <col width="55.81640625" customWidth="1" style="46" min="8" max="8"/>
+    <col width="58.1796875" customWidth="1" style="65" min="9" max="9"/>
+    <col width="43.453125" customWidth="1" style="65" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="65" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="46" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="46" min="13" max="13"/>
+    <col width="14.81640625" customWidth="1" style="46" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="46" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="46" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -39764,7 +39764,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="89.45" customHeight="1">
+    <row r="5" ht="89.5" customHeight="1">
       <c r="A5" s="43" t="n"/>
       <c r="B5" s="127" t="n">
         <v>1</v>
@@ -40377,24 +40377,24 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="25.42578125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="61.42578125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="47.85546875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="2" min="33" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="25.453125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="61.453125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="47.81640625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.81640625" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -41206,24 +41206,24 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="9.140625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="9.1796875" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
     <col width="24" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="69.85546875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="36.85546875" customWidth="1" style="2" min="7" max="7"/>
-    <col width="61.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="66.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="48.140625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="11.140625" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="14.7109375" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="2" min="33" max="16384"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="69.81640625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="36.81640625" customWidth="1" style="2" min="7" max="7"/>
+    <col width="61.54296875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="66.453125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="48.1796875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="11.1796875" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="14.7265625" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -43086,24 +43086,24 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
   <cols>
-    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
-    <col width="9.140625" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="17.5703125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
-    <col width="65.5703125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="40.28515625" customWidth="1" style="2" min="7" max="7"/>
-    <col width="53.85546875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="66.42578125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="46.28515625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="11.28515625" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
-    <col width="14.140625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="32"/>
-    <col width="8.7109375" customWidth="1" style="2" min="33" max="16384"/>
+    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
+    <col width="9.1796875" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="17.54296875" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
+    <col width="65.54296875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="40.26953125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="53.81640625" customWidth="1" style="2" min="8" max="8"/>
+    <col width="66.453125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="46.26953125" customWidth="1" style="1" min="10" max="10"/>
+    <col width="11.26953125" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
+    <col width="14.1796875" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
+    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>

</xml_diff>

<commit_message>
Only two unwritten services left
</commit_message>
<xml_diff>
--- a/PythonProject/gui/Remote_Services.xlsx
+++ b/PythonProject/gui/Remote_Services.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="779" firstSheet="19" activeTab="22" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-105" yWindow="0" windowWidth="22470" windowHeight="15585" tabRatio="779" firstSheet="19" activeTab="22" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demo Mode" sheetId="1" state="visible" r:id="rId1"/>
@@ -10733,22 +10733,22 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col width="3.26953125" customWidth="1" min="1" max="1"/>
-    <col width="6.81640625" customWidth="1" min="2" max="2"/>
-    <col width="16.26953125" customWidth="1" min="3" max="3"/>
-    <col width="14.453125" customWidth="1" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
-    <col width="37.26953125" customWidth="1" min="6" max="6"/>
-    <col width="48.54296875" customWidth="1" min="7" max="7"/>
-    <col width="55.1796875" customWidth="1" min="8" max="8"/>
-    <col width="39.453125" customWidth="1" min="9" max="9"/>
+    <col width="3.28515625" customWidth="1" min="1" max="1"/>
+    <col width="6.85546875" customWidth="1" min="2" max="2"/>
+    <col width="16.28515625" customWidth="1" min="3" max="3"/>
+    <col width="14.42578125" customWidth="1" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
+    <col width="37.28515625" customWidth="1" min="6" max="6"/>
+    <col width="48.5703125" customWidth="1" min="7" max="7"/>
+    <col width="55.140625" customWidth="1" min="8" max="8"/>
+    <col width="39.42578125" customWidth="1" min="9" max="9"/>
     <col width="47" customWidth="1" min="10" max="10"/>
-    <col width="14.54296875" customWidth="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" min="13" max="13"/>
-    <col width="13.26953125" customWidth="1" min="14" max="14"/>
+    <col width="14.5703125" customWidth="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="13.28515625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -11654,24 +11654,24 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="56.453125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="54.1796875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="17.54296875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="56.42578125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="54.140625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="17.5703125" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="2" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -12801,22 +12801,22 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col width="2.81640625" customWidth="1" min="1" max="1"/>
-    <col width="6.1796875" customWidth="1" style="12" min="2" max="2"/>
+    <col width="2.85546875" customWidth="1" min="1" max="1"/>
+    <col width="6.140625" customWidth="1" style="12" min="2" max="2"/>
     <col width="19" customWidth="1" style="12" min="3" max="3"/>
-    <col width="24.81640625" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
-    <col width="34.1796875" customWidth="1" min="6" max="6"/>
-    <col width="46.1796875" customWidth="1" min="7" max="7"/>
-    <col width="39.7265625" customWidth="1" min="8" max="8"/>
-    <col width="58.1796875" customWidth="1" style="12" min="9" max="9"/>
-    <col width="61.26953125" customWidth="1" style="12" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" min="13" max="13"/>
-    <col width="17.7265625" customWidth="1" min="14" max="14"/>
+    <col width="24.85546875" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
+    <col width="34.140625" customWidth="1" min="6" max="6"/>
+    <col width="46.140625" customWidth="1" min="7" max="7"/>
+    <col width="39.7109375" customWidth="1" min="8" max="8"/>
+    <col width="58.140625" customWidth="1" style="12" min="9" max="9"/>
+    <col width="61.28515625" customWidth="1" style="12" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="12" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="17.7109375" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -13733,22 +13733,22 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col width="3" customWidth="1" min="1" max="1"/>
-    <col width="7.1796875" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
-    <col width="22.453125" customWidth="1" style="12" min="3" max="3"/>
-    <col width="9.81640625" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
-    <col width="52.1796875" customWidth="1" min="6" max="6"/>
-    <col width="41.81640625" customWidth="1" min="7" max="7"/>
-    <col width="45.81640625" customWidth="1" min="8" max="8"/>
-    <col width="53.1796875" customWidth="1" style="12" min="9" max="9"/>
-    <col width="47.1796875" customWidth="1" style="12" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" min="13" max="13"/>
-    <col width="15.453125" customWidth="1" min="14" max="14"/>
+    <col width="7.140625" bestFit="1" customWidth="1" style="12" min="2" max="2"/>
+    <col width="22.42578125" customWidth="1" style="12" min="3" max="3"/>
+    <col width="9.85546875" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
+    <col width="52.140625" customWidth="1" min="6" max="6"/>
+    <col width="41.85546875" customWidth="1" min="7" max="7"/>
+    <col width="45.85546875" customWidth="1" min="8" max="8"/>
+    <col width="53.140625" customWidth="1" style="12" min="9" max="9"/>
+    <col width="47.140625" customWidth="1" style="12" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="12" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="15.42578125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -15581,28 +15581,28 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="2.453125" customWidth="1" style="2" min="1" max="1"/>
-    <col width="6.1796875" customWidth="1" style="2" min="2" max="2"/>
-    <col width="21.81640625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="18.453125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="68.1796875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="43.7265625" customWidth="1" style="2" min="7" max="7"/>
-    <col width="50.54296875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.81640625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="53.1796875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" min="13" max="13"/>
-    <col width="16.81640625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
+    <col width="2.42578125" customWidth="1" style="2" min="1" max="1"/>
+    <col width="6.140625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="21.85546875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="18.42578125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="68.140625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="43.7109375" customWidth="1" style="2" min="7" max="7"/>
+    <col width="50.5703125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.85546875" customWidth="1" style="1" min="9" max="9"/>
+    <col width="53.140625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="2" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -16561,24 +16561,24 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="60.1796875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="48.81640625" customWidth="1" style="2" min="7" max="7"/>
-    <col width="60.1796875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="60.140625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="48.85546875" customWidth="1" style="2" min="7" max="7"/>
+    <col width="60.140625" customWidth="1" style="2" min="8" max="8"/>
     <col width="63" customWidth="1" style="1" min="9" max="9"/>
-    <col width="49.1796875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.81640625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
+    <col width="49.140625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="2" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -17489,24 +17489,24 @@
   </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col width="2.81640625" customWidth="1" min="1" max="1"/>
+    <col width="2.85546875" customWidth="1" min="1" max="1"/>
     <col width="26" customWidth="1" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
-    <col width="42.81640625" customWidth="1" min="6" max="6"/>
-    <col width="47.54296875" customWidth="1" min="7" max="7"/>
-    <col width="38.81640625" customWidth="1" min="8" max="8"/>
-    <col width="37.453125" customWidth="1" min="9" max="9"/>
-    <col width="50.81640625" customWidth="1" min="10" max="10"/>
-    <col width="17.54296875" customWidth="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" min="13" max="13"/>
-    <col width="18.1796875" customWidth="1" min="14" max="14"/>
+    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
+    <col width="42.85546875" customWidth="1" min="6" max="6"/>
+    <col width="47.5703125" customWidth="1" min="7" max="7"/>
+    <col width="38.85546875" customWidth="1" min="8" max="8"/>
+    <col width="37.42578125" customWidth="1" min="9" max="9"/>
+    <col width="50.85546875" customWidth="1" min="10" max="10"/>
+    <col width="17.5703125" customWidth="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="18.140625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -18105,24 +18105,24 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="56.453125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="45.7265625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="20.453125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="56.42578125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="45.7109375" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="20.42578125" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="2" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -18541,24 +18541,24 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="43" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="80" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
-    <col width="55.54296875" customWidth="1" style="43" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="43" min="7" max="7"/>
-    <col width="58.54296875" customWidth="1" style="43" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="44" min="9" max="9"/>
-    <col width="47.81640625" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
-    <col width="16.54296875" customWidth="1" style="43" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="43" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="43" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="43" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="80" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
+    <col width="55.5703125" customWidth="1" style="43" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="43" min="7" max="7"/>
+    <col width="58.5703125" customWidth="1" style="43" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="44" min="9" max="9"/>
+    <col width="47.85546875" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
+    <col width="16.5703125" customWidth="1" style="43" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="43" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="43" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -19024,24 +19024,24 @@
       <selection activeCell="J5" sqref="B5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="47.7265625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.1796875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="47.7109375" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.140625" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="2" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -20106,21 +20106,21 @@
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col width="3.26953125" customWidth="1" min="1" max="1"/>
-    <col width="6.54296875" customWidth="1" min="2" max="2"/>
-    <col width="9.1796875" customWidth="1" min="3" max="3"/>
-    <col width="13.26953125" customWidth="1" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
-    <col width="47.7265625" customWidth="1" min="6" max="6"/>
-    <col width="44.26953125" customWidth="1" min="7" max="7"/>
-    <col width="49.1796875" customWidth="1" min="8" max="8"/>
-    <col width="47.1796875" customWidth="1" min="9" max="10"/>
-    <col width="16.81640625" customWidth="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" min="13" max="13"/>
-    <col width="15.81640625" customWidth="1" min="14" max="14"/>
+    <col width="3.28515625" customWidth="1" min="1" max="1"/>
+    <col width="6.5703125" customWidth="1" min="2" max="2"/>
+    <col width="9.140625" customWidth="1" min="3" max="3"/>
+    <col width="13.28515625" customWidth="1" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
+    <col width="47.7109375" customWidth="1" min="6" max="6"/>
+    <col width="44.28515625" customWidth="1" min="7" max="7"/>
+    <col width="49.140625" customWidth="1" min="8" max="8"/>
+    <col width="47.140625" customWidth="1" min="9" max="10"/>
+    <col width="16.85546875" customWidth="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="15.85546875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -20816,24 +20816,24 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
+    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
     <col width="19" customWidth="1" style="80" min="3" max="3"/>
-    <col width="18.54296875" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
-    <col width="60.1796875" customWidth="1" style="43" min="6" max="6"/>
-    <col width="48.81640625" customWidth="1" style="43" min="7" max="7"/>
-    <col width="78.26953125" customWidth="1" style="43" min="8" max="8"/>
-    <col width="52.26953125" customWidth="1" style="44" min="9" max="9"/>
-    <col width="43.54296875" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
-    <col width="18.7265625" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="46" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="46" min="34" max="16384"/>
+    <col width="18.5703125" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
+    <col width="60.140625" customWidth="1" style="43" min="6" max="6"/>
+    <col width="48.85546875" customWidth="1" style="43" min="7" max="7"/>
+    <col width="78.28515625" customWidth="1" style="43" min="8" max="8"/>
+    <col width="52.28515625" customWidth="1" style="44" min="9" max="9"/>
+    <col width="43.5703125" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
+    <col width="18.7109375" customWidth="1" style="46" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="46" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -23635,21 +23635,21 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="42.1796875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.453125" customWidth="1" min="14" max="14"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="42.140625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.42578125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -24012,21 +24012,21 @@
       <selection activeCell="E16" sqref="D16:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
     <col width="47" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.81640625" customWidth="1" min="14" max="14"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.85546875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -24323,20 +24323,20 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col width="2" customWidth="1" min="1" max="1"/>
-    <col width="16.1796875" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13.1796875" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
+    <col width="16.140625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.140625" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
     <col width="44" customWidth="1" style="12" min="6" max="6"/>
-    <col width="51.81640625" customWidth="1" style="12" min="7" max="7"/>
-    <col width="41.54296875" customWidth="1" style="12" min="8" max="8"/>
+    <col width="51.85546875" customWidth="1" style="12" min="7" max="7"/>
+    <col width="41.5703125" customWidth="1" style="12" min="8" max="8"/>
     <col width="45" customWidth="1" style="12" min="9" max="9"/>
-    <col width="47.81640625" customWidth="1" style="12" min="10" max="10"/>
+    <col width="47.85546875" customWidth="1" style="12" min="10" max="10"/>
     <col width="14" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" min="13" max="13"/>
+    <col width="19.42578125" customWidth="1" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" min="13" max="13"/>
     <col width="16" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
@@ -24998,28 +24998,28 @@
   </sheetPr>
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G14" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="57.7265625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="54.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="60.1796875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="60.453125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="48.1796875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.453125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="57.7109375" customWidth="1" style="2" min="6" max="6"/>
+    <col width="54.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="60.140625" customWidth="1" style="2" min="8" max="8"/>
+    <col width="60.42578125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="48.140625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.42578125" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="2" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -25917,21 +25917,21 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="67.81640625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="67.85546875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
     <col width="46" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.1796875" customWidth="1" min="14" max="14"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.140625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -26503,25 +26503,25 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D5" sqref="D5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="40.7265625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.26953125" customWidth="1" min="14" max="14"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="40.7109375" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.28515625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -27226,26 +27226,26 @@
   </sheetPr>
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col width="3.26953125" customWidth="1" min="1" max="1"/>
-    <col width="6.81640625" customWidth="1" min="2" max="2"/>
-    <col width="20.54296875" customWidth="1" min="3" max="3"/>
-    <col width="13.453125" customWidth="1" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="32" min="5" max="5"/>
-    <col width="37.26953125" customWidth="1" min="6" max="6"/>
-    <col width="48.54296875" customWidth="1" min="7" max="7"/>
-    <col width="55.1796875" customWidth="1" min="8" max="8"/>
-    <col width="36.7265625" customWidth="1" min="9" max="9"/>
-    <col width="50.26953125" customWidth="1" min="10" max="10"/>
-    <col width="14.54296875" customWidth="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" min="13" max="13"/>
-    <col width="17.7265625" customWidth="1" min="14" max="14"/>
+    <col width="3.28515625" customWidth="1" min="1" max="1"/>
+    <col width="6.85546875" customWidth="1" min="2" max="2"/>
+    <col width="20.5703125" customWidth="1" min="3" max="3"/>
+    <col width="13.42578125" customWidth="1" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="32" min="5" max="5"/>
+    <col width="37.28515625" customWidth="1" min="6" max="6"/>
+    <col width="48.5703125" customWidth="1" min="7" max="7"/>
+    <col width="55.140625" customWidth="1" min="8" max="8"/>
+    <col width="36.7109375" customWidth="1" min="9" max="9"/>
+    <col width="50.28515625" customWidth="1" min="10" max="10"/>
+    <col width="14.5703125" customWidth="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="17.7109375" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
@@ -28436,24 +28436,24 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="80" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
-    <col width="55.54296875" customWidth="1" style="43" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="43" min="7" max="7"/>
-    <col width="58.54296875" customWidth="1" style="43" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="44" min="9" max="9"/>
-    <col width="42.26953125" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
+    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="80" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
+    <col width="55.5703125" customWidth="1" style="43" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="43" min="7" max="7"/>
+    <col width="58.5703125" customWidth="1" style="43" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="44" min="9" max="9"/>
+    <col width="42.28515625" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="14" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="46" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="46" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="46" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -28749,21 +28749,21 @@
       <selection activeCell="F5" sqref="F5:J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="90.1796875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="58.54296875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="47.81640625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.26953125" customWidth="1" min="14" max="14"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="90.140625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="58.5703125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="47.85546875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.28515625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -29343,21 +29343,21 @@
       <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="28.54296875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="40.453125" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="60.81640625" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="28.5703125" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="40.42578125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="60.85546875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
     <col width="41" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.1796875" customWidth="1" min="14" max="14"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.140625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -33037,21 +33037,21 @@
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="60.1796875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="48.81640625" customWidth="1" style="2" min="7" max="7"/>
-    <col width="78.26953125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="60.140625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="48.85546875" customWidth="1" style="2" min="7" max="7"/>
+    <col width="78.28515625" customWidth="1" style="2" min="8" max="8"/>
     <col width="57" customWidth="1" style="1" min="9" max="9"/>
     <col width="45" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="16.1796875" customWidth="1" min="14" max="14"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="16.140625" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -34115,21 +34115,21 @@
       <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="11.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="14.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="15.54296875" customWidth="1" style="36" min="5" max="5"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="11.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="15.5703125" customWidth="1" style="36" min="5" max="5"/>
     <col width="86" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
     <col width="65" customWidth="1" style="2" min="8" max="8"/>
-    <col width="58.453125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="49.1796875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="17.453125" customWidth="1" min="14" max="14"/>
+    <col width="58.42578125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="49.140625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="17.42578125" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -38381,24 +38381,24 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="43" min="2" max="2"/>
+    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="43" min="2" max="2"/>
     <col width="19" customWidth="1" style="80" min="3" max="3"/>
-    <col width="18.54296875" customWidth="1" style="43" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="81" min="5" max="5"/>
-    <col width="60.1796875" customWidth="1" style="43" min="6" max="6"/>
-    <col width="48.81640625" customWidth="1" style="43" min="7" max="7"/>
-    <col width="85.54296875" customWidth="1" style="43" min="8" max="8"/>
+    <col width="18.5703125" customWidth="1" style="43" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="81" min="5" max="5"/>
+    <col width="60.140625" customWidth="1" style="43" min="6" max="6"/>
+    <col width="48.85546875" customWidth="1" style="43" min="7" max="7"/>
+    <col width="85.5703125" customWidth="1" style="43" min="8" max="8"/>
     <col width="63" customWidth="1" style="44" min="9" max="9"/>
-    <col width="38.1796875" customWidth="1" style="44" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="44" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="43" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="43" min="13" max="13"/>
-    <col width="15.54296875" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="46" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="46" min="34" max="16384"/>
+    <col width="38.140625" customWidth="1" style="44" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="44" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
+    <col width="15.5703125" customWidth="1" style="46" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="46" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -39029,21 +39029,21 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col width="10.26953125" customWidth="1" style="12" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="12" min="3" max="3"/>
-    <col width="15.453125" customWidth="1" style="12" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="39" min="5" max="5"/>
-    <col width="52.7265625" customWidth="1" min="6" max="6"/>
-    <col width="51.1796875" customWidth="1" min="7" max="7"/>
-    <col width="55.81640625" customWidth="1" min="8" max="8"/>
-    <col width="58.1796875" customWidth="1" style="12" min="9" max="9"/>
-    <col width="45.1796875" customWidth="1" style="12" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="12" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" min="13" max="13"/>
-    <col width="17.81640625" customWidth="1" min="14" max="14"/>
+    <col width="10.28515625" customWidth="1" style="12" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="12" min="3" max="3"/>
+    <col width="15.42578125" customWidth="1" style="12" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="39" min="5" max="5"/>
+    <col width="52.7109375" customWidth="1" min="6" max="6"/>
+    <col width="51.140625" customWidth="1" min="7" max="7"/>
+    <col width="55.85546875" customWidth="1" min="8" max="8"/>
+    <col width="58.140625" customWidth="1" style="12" min="9" max="9"/>
+    <col width="45.140625" customWidth="1" style="12" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="12" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="17.85546875" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -39616,24 +39616,24 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="46" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="65" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="65" min="3" max="3"/>
-    <col width="15.453125" customWidth="1" style="65" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="66" min="5" max="5"/>
-    <col width="52.7265625" customWidth="1" style="46" min="6" max="6"/>
-    <col width="51.1796875" customWidth="1" style="46" min="7" max="7"/>
-    <col width="55.81640625" customWidth="1" style="46" min="8" max="8"/>
-    <col width="58.1796875" customWidth="1" style="65" min="9" max="9"/>
-    <col width="43.453125" customWidth="1" style="65" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="65" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="46" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="46" min="13" max="13"/>
-    <col width="14.81640625" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="46" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="46" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="65" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="65" min="3" max="3"/>
+    <col width="15.42578125" customWidth="1" style="65" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="66" min="5" max="5"/>
+    <col width="52.7109375" customWidth="1" style="46" min="6" max="6"/>
+    <col width="51.140625" customWidth="1" style="46" min="7" max="7"/>
+    <col width="55.85546875" customWidth="1" style="46" min="8" max="8"/>
+    <col width="58.140625" customWidth="1" style="65" min="9" max="9"/>
+    <col width="43.42578125" customWidth="1" style="65" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="65" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="46" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="46" min="13" max="13"/>
+    <col width="14.85546875" customWidth="1" style="46" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="46" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -39764,7 +39764,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="89.5" customHeight="1">
+    <row r="5" ht="89.45" customHeight="1">
       <c r="A5" s="43" t="n"/>
       <c r="B5" s="127" t="n">
         <v>1</v>
@@ -40377,24 +40377,24 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
-    <col width="10.26953125" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="25.453125" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="55.54296875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="50.453125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="61.453125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="56.26953125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="47.81640625" customWidth="1" style="1" min="10" max="10"/>
-    <col width="13.1796875" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="15.81640625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
+    <col width="10.28515625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="25.42578125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="55.5703125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="50.42578125" customWidth="1" style="2" min="7" max="7"/>
+    <col width="61.42578125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="56.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="47.85546875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="13.140625" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="15.85546875" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="2" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -41206,24 +41206,24 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
-    <col width="9.1796875" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
+    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
+    <col width="9.140625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
     <col width="24" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="69.81640625" customWidth="1" style="2" min="6" max="6"/>
-    <col width="36.81640625" customWidth="1" style="2" min="7" max="7"/>
-    <col width="61.54296875" customWidth="1" style="2" min="8" max="8"/>
-    <col width="66.453125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="48.1796875" customWidth="1" style="1" min="10" max="10"/>
-    <col width="11.1796875" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="14.7265625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="69.85546875" customWidth="1" style="2" min="6" max="6"/>
+    <col width="36.85546875" customWidth="1" style="2" min="7" max="7"/>
+    <col width="61.5703125" customWidth="1" style="2" min="8" max="8"/>
+    <col width="66.42578125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="48.140625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="11.140625" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="14.7109375" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="2" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -43086,24 +43086,24 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
   <cols>
-    <col width="8.7265625" customWidth="1" style="2" min="1" max="1"/>
-    <col width="9.1796875" customWidth="1" style="2" min="2" max="2"/>
-    <col width="15.1796875" customWidth="1" style="8" min="3" max="3"/>
-    <col width="17.54296875" customWidth="1" style="2" min="4" max="4"/>
-    <col width="11.26953125" customWidth="1" style="36" min="5" max="5"/>
-    <col width="65.54296875" customWidth="1" style="2" min="6" max="6"/>
-    <col width="40.26953125" customWidth="1" style="2" min="7" max="7"/>
-    <col width="53.81640625" customWidth="1" style="2" min="8" max="8"/>
-    <col width="66.453125" customWidth="1" style="1" min="9" max="9"/>
-    <col width="46.26953125" customWidth="1" style="1" min="10" max="10"/>
-    <col width="11.26953125" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.453125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="18.81640625" customWidth="1" style="2" min="13" max="13"/>
-    <col width="14.1796875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7265625" customWidth="1" style="2" min="15" max="33"/>
-    <col width="8.7265625" customWidth="1" style="2" min="34" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="1" max="1"/>
+    <col width="9.140625" customWidth="1" style="2" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" style="8" min="3" max="3"/>
+    <col width="17.5703125" customWidth="1" style="2" min="4" max="4"/>
+    <col width="11.28515625" customWidth="1" style="36" min="5" max="5"/>
+    <col width="65.5703125" customWidth="1" style="2" min="6" max="6"/>
+    <col width="40.28515625" customWidth="1" style="2" min="7" max="7"/>
+    <col width="53.85546875" customWidth="1" style="2" min="8" max="8"/>
+    <col width="66.42578125" customWidth="1" style="1" min="9" max="9"/>
+    <col width="46.28515625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="11.28515625" bestFit="1" customWidth="1" style="1" min="11" max="11"/>
+    <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
+    <col width="14.140625" customWidth="1" style="2" min="14" max="14"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="36"/>
+    <col width="8.7109375" customWidth="1" style="2" min="37" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>

</xml_diff>

<commit_message>
Before swapping service details formatting
</commit_message>
<xml_diff>
--- a/PythonProject/gui/Remote_Services.xlsx
+++ b/PythonProject/gui/Remote_Services.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="778" firstSheet="9" activeTab="11" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="778" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demo Mode" sheetId="1" state="visible" r:id="rId1"/>
@@ -12071,8 +12071,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="17.5703125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="2" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="2" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -14015,8 +14015,8 @@
   </sheetPr>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -14351,14 +14351,11 @@
       <c r="G8" s="53" t="inlineStr">
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT" page 
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT )</t>
-        </is>
-      </c>
-      <c r="H8" s="53" t="inlineStr">
-        <is>
-          <t>• The vehicle should support rear seat heating</t>
-        </is>
-      </c>
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT )
+• The vehicle should support rear seat heating</t>
+        </is>
+      </c>
+      <c r="H8" s="53" t="n"/>
       <c r="I8" s="53" t="inlineStr">
         <is>
           <t>In 'MY CABIN COMFORT', Go to 'Quick start' tab and enable 'Interior surface heating' option</t>
@@ -14379,7 +14376,7 @@
       <c r="M8" s="53" t="n"/>
       <c r="N8" s="72" t="n"/>
     </row>
-    <row r="9" ht="141.75" customHeight="1">
+    <row r="9" ht="160.5" customHeight="1">
       <c r="A9" s="2" t="n"/>
       <c r="B9" s="50" t="n">
         <v>5</v>
@@ -14407,14 +14404,11 @@
       <c r="G9" s="53" t="inlineStr">
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Quick start" page 
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start )</t>
-        </is>
-      </c>
-      <c r="H9" s="53" t="inlineStr">
-        <is>
-          <t>• The vehicle should support rear seat heating</t>
-        </is>
-      </c>
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start )
+• The vehicle should support rear seat heating</t>
+        </is>
+      </c>
+      <c r="H9" s="53" t="n"/>
       <c r="I9" s="53" t="inlineStr">
         <is>
           <t>1. Try to set the Target Temperature Bar to some desired value in the range between 16degC to 26degC with 1degC increments / decrements</t>
@@ -14459,14 +14453,14 @@
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Quick start" page 
 ( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start )
+• The vehicle should support rear seat heating
+• Make sure at least 30% of Fuel to be present in Fuel Tank
 Note : "MY CABIN COMFORT" Quick start activates only for 30 mins</t>
         </is>
       </c>
       <c r="H10" s="53" t="inlineStr">
         <is>
-          <t>• The vehicle should support rear seat heating
-• Make sure at least 30% of Fuel to be present in Fuel Tank
-• Vehicle Ignition = Off</t>
+          <t>• Vehicle Ignition = Off</t>
         </is>
       </c>
       <c r="I10" s="53" t="inlineStr">
@@ -14531,14 +14525,14 @@
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Quick start" page 
 ( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start ) 
+• The vehicle should support rear seat heating
+• Make sure at least 30% of Fuel to be present in Fuel Tank
 Note : "MY CABIN COMFORT" Quick start activates only for 30 mins</t>
         </is>
       </c>
       <c r="H11" s="53" t="inlineStr">
         <is>
-          <t>• The vehicle should support rear seat heating
-• Make sure at least 30% of Fuel to be present in Fuel Tank
-• Vehicle Ignition = Off</t>
+          <t>• Vehicle Ignition = Off</t>
         </is>
       </c>
       <c r="I11" s="53" t="inlineStr">
@@ -14610,14 +14604,14 @@
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Quick start" page 
 ( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start )
+• The vehicle should support rear seat heating
+• Make sure at least 30% of Fuel to be present in Fuel Tank
 Note : "MY CABIN COMFORT" Quick start activates only for 30 mins</t>
         </is>
       </c>
       <c r="H12" s="53" t="inlineStr">
         <is>
-          <t>• The vehicle should support rear seat heating
-• Vehicle Ignition = Off
-• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
+          <t>• Vehicle Ignition = Off</t>
         </is>
       </c>
       <c r="I12" s="53" t="inlineStr">
@@ -14689,14 +14683,14 @@
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Quick start" page 
 ( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start )
+• The vehicle should support rear seat heating
+• Make sure at least 30% of Fuel to be present in Fuel Tank
 Note : "MY CABIN COMFORT" Quick start activates only for 30 mins</t>
         </is>
       </c>
       <c r="H13" s="53" t="inlineStr">
         <is>
-          <t>• The vehicle should support rear seat heating
-• Vehicle Ignition = Off
-• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
+          <t>• Vehicle Ignition = Off</t>
         </is>
       </c>
       <c r="I13" s="53" t="inlineStr">
@@ -14768,14 +14762,14 @@
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Quick start" page 
 ( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start )
+• The vehicle should support rear seat heating
+• Make sure at least 30% of Fuel to be present in Fuel Tank
 Note : "MY CABIN COMFORT" Quick start activates only for 30 mins</t>
         </is>
       </c>
       <c r="H14" s="53" t="inlineStr">
         <is>
-          <t>• The vehicle should support rear seat heating
-• Vehicle Ignition = Off
-• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
+          <t>• Vehicle Ignition = Off</t>
         </is>
       </c>
       <c r="I14" s="53" t="inlineStr">
@@ -14846,15 +14840,15 @@
       <c r="G15" s="53" t="inlineStr">
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Quick start" page 
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start )
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start ) 
+• The vehicle should support rear seat heating
+• Make sure at least 30% of Fuel to be present in Fuel Tank
 Note : "MY CABIN COMFORT" Quick start activates only for 30 mins</t>
         </is>
       </c>
       <c r="H15" s="53" t="inlineStr">
         <is>
-          <t>• The vehicle should support rear seat heating
-• Vehicle Ignition = Off
-• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
+          <t>• Vehicle Ignition = Off</t>
         </is>
       </c>
       <c r="I15" s="53" t="inlineStr">
@@ -14904,7 +14898,7 @@
       <c r="M15" s="53" t="n"/>
       <c r="N15" s="72" t="n"/>
     </row>
-    <row r="16" ht="189" customHeight="1">
+    <row r="16" ht="212.25" customHeight="1">
       <c r="A16" s="2" t="n"/>
       <c r="B16" s="50" t="n">
         <v>12</v>
@@ -14933,14 +14927,14 @@
         <is>
           <t>• "MY CABIN COMFORT" is active
 • The screen focus is in "MY CABIN COMFORT - Quick start" page 
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start )</t>
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Quick start )
+• The vehicle should support rear seat heating
+• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
         </is>
       </c>
       <c r="H16" s="53" t="inlineStr">
         <is>
-          <t>• The vehicle should support rear seat heating
-• Vehicle Ignition = Off
-• Make sure at least 30% of Fuel to be present in Fuel Tank
+          <t>• Vehicle Ignition = Off
 • Interior surface heating = On
 • 'Front Driver Seat Heating' = Active
 • 'Front Passenger Seat Heating' = Active
@@ -15046,14 +15040,11 @@
       <c r="G18" s="53" t="inlineStr">
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Set timer" page 
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Set timer )</t>
-        </is>
-      </c>
-      <c r="H18" s="53" t="inlineStr">
-        <is>
-          <t>• The vehicle should support rear seat heating</t>
-        </is>
-      </c>
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Set timer )
+• The vehicle should support rear seat heating</t>
+        </is>
+      </c>
+      <c r="H18" s="53" t="n"/>
       <c r="I18" s="53" t="inlineStr">
         <is>
           <t>In 'MY CABIN COMFORT - Set timer' tab , Click on 'SETTINGS' &amp; Observe</t>
@@ -15106,13 +15097,13 @@
       <c r="G19" s="53" t="inlineStr">
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Set timer" page 
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Set timer )</t>
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Set timer )
+• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
         </is>
       </c>
       <c r="H19" s="53" t="inlineStr">
         <is>
-          <t>• Ignition = Off
-• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
+          <t>• Ignition = Off</t>
         </is>
       </c>
       <c r="I19" s="53" t="inlineStr">
@@ -15176,13 +15167,13 @@
       <c r="G20" s="53" t="inlineStr">
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Set timer" page 
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Set timer )</t>
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Set timer )
+• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
         </is>
       </c>
       <c r="H20" s="53" t="inlineStr">
         <is>
           <t>• Ignition = Off
-• Make sure at least 30% of Fuel to be present in Fuel Tank
 • Make sure particular Seat Heating / Cooling is selected(Ex : Front Driver Seat , Front Passenger Seat , Rear Passenger Seats ....etc.)</t>
         </is>
       </c>
@@ -15523,7 +15514,7 @@
       <c r="M25" s="53" t="n"/>
       <c r="N25" s="134" t="n"/>
     </row>
-    <row r="26" ht="141.75" customHeight="1">
+    <row r="26" ht="165.75" customHeight="1">
       <c r="B26" s="50" t="n">
         <v>22</v>
       </c>
@@ -15550,13 +15541,13 @@
       <c r="G26" s="53" t="inlineStr">
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Set timer" page 
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Set timer )</t>
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Set timer )
+• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
         </is>
       </c>
       <c r="H26" s="53" t="inlineStr">
         <is>
-          <t>• Ignition = Off
-• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
+          <t>• Ignition = Off</t>
         </is>
       </c>
       <c r="I26" s="53" t="inlineStr">
@@ -15610,13 +15601,13 @@
       <c r="G27" s="53" t="inlineStr">
         <is>
           <t>• The screen focus is in "MY CABIN COMFORT - Set timer" page 
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Set timer )</t>
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; CAR REMOTE --&gt; MY CABIN COMFORT --&gt; Set timer )
+• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
         </is>
       </c>
       <c r="H27" s="53" t="inlineStr">
         <is>
-          <t>• Ignition = Off
-• Make sure at least 30% of Fuel to be present in Fuel Tank</t>
+          <t>• Ignition = Off</t>
         </is>
       </c>
       <c r="I27" s="53" t="inlineStr">
@@ -15836,8 +15827,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" min="13" max="13"/>
     <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="2" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="2" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -16743,8 +16734,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="2" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="2" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -18287,8 +18278,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="20.42578125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="2" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="2" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -18723,8 +18714,8 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="16.5703125" customWidth="1" style="43" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="43" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="43" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="43" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="43" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -19206,8 +19197,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="15.140625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="2" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="2" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -20978,7 +20969,7 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -20998,8 +20989,8 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="18.7109375" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="46" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="46" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -25071,8 +25062,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="15.42578125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="2" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="2" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -28505,8 +28496,8 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="14" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="46" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="46" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -38844,8 +38835,8 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="15.5703125" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="46" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="46" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -40074,8 +40065,8 @@
     <col width="19.42578125" customWidth="1" style="46" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="46" min="13" max="13"/>
     <col width="14.85546875" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="46" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="46" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -40835,8 +40826,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="15.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="2" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="2" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -41652,8 +41643,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="14.7109375" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="2" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="2" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
@@ -43546,8 +43537,8 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="14.140625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="44"/>
-    <col width="8.7109375" customWidth="1" style="2" min="45" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="45"/>
+    <col width="8.7109375" customWidth="1" style="2" min="46" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>

</xml_diff>

<commit_message>
Getting ready for first testrun
</commit_message>
<xml_diff>
--- a/PythonProject/gui/Remote_Services.xlsx
+++ b/PythonProject/gui/Remote_Services.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="778" firstSheet="19" activeTab="29" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="778" firstSheet="5" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demo Mode" sheetId="1" state="visible" r:id="rId1"/>
@@ -157,7 +157,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -191,6 +191,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -621,7 +627,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="254">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -1277,6 +1283,36 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1333,7 +1369,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
-  <dxfs count="533">
+  <dxfs count="529">
     <dxf>
       <font>
         <b val="1"/>
@@ -4759,67 +4795,33 @@
     <dxf>
       <font>
         <b val="1"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
         <strike val="0"/>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.5999633777886288"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.1498764000366222"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="2" tint="-0.749961851863155"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <strike val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -4843,17 +4845,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.249946592608417"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -8078,7 +8069,7 @@
       <col>1</col>
       <colOff>554703</colOff>
       <row>1</row>
-      <rowOff>354945</rowOff>
+      <rowOff>358120</rowOff>
     </to>
     <pic>
       <nvPicPr>
@@ -11054,45 +11045,45 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Demo Mode</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Pre Condition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • My Bentley App must be installed in the mobile phone successfully.</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -11971,39 +11962,39 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="17.5703125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="2" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="2" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Remote Honk &amp; Flash</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -12014,13 +12005,13 @@
 • Ignition = OFF &amp; Engine = OFF</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -13098,8 +13089,8 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="D11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -13136,34 +13127,34 @@
     </row>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="n"/>
-      <c r="B2" s="231" t="inlineStr">
+      <c r="B2" s="241" t="inlineStr">
         <is>
           <t>My Car Statistics</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="232" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="242" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="2" t="n"/>
-      <c r="B3" s="233" t="inlineStr">
+      <c r="B3" s="243" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="225" t="n"/>
-      <c r="D3" s="233" t="n"/>
+      <c r="C3" s="235" t="n"/>
+      <c r="D3" s="243" t="n"/>
       <c r="E3" s="48" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t xml:space="preserve">Ensure that below preconditions are met before start the testing for this service
 • This service applicable for only on PHEV models
@@ -13176,13 +13167,13 @@
 </t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" s="2" t="inlineStr"/>
@@ -13698,79 +13689,32 @@
       </c>
       <c r="C13" s="51" t="inlineStr">
         <is>
-          <t>EUR, NAR, CHN</t>
-        </is>
-      </c>
-      <c r="D13" s="51" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="E13" s="52" t="n">
-        <v>7</v>
-      </c>
-      <c r="F13" s="53" t="inlineStr">
-        <is>
-          <t>Verify Single Service Activation / Deactivation of 'My Car Statistics' service in SERVICE MANAGEMENT screen</t>
-        </is>
-      </c>
-      <c r="G13" s="53" t="inlineStr">
-        <is>
-          <t>• The screen focus is in "My Bentley App - SERVICE MANAGEMENT" page
-(My Bentley App --&gt;SIGN IN --&gt; Vehicle "DASHBOARD" Screen --&gt;  Select "i" icon --&gt; SERVICE MANAGEMENT screen)</t>
-        </is>
-      </c>
-      <c r="H13" s="53" t="n"/>
-      <c r="I13" s="53" t="inlineStr">
-        <is>
-          <t>1. In 'SERVICE MANAGEMENT' screen,  Select 'MY CAR STATISTICS' = Activate / Deactivate
-2. Go to CAR REMOTE screen and check the 'MY CAR STATISTICS' section</t>
-        </is>
-      </c>
-      <c r="J13" s="77" t="inlineStr">
-        <is>
-          <t>In My Bentley App, Under 'CAR REMOTE' screen
-1. MY CAR STATISTICS = Deactivate --&gt; 'MY CAR STATISTICS' Service should not be accessible under CAR REMOTE Screen(i.e. Under CAR REMOTE screen , 'MY CAR STATISTICS' section should be greyed out and should display 'Function disabled' text)
-2. MY CAR STATISTICS = Activate --&gt; 'MY CAR STATISTICS' Service should be active and accessible under CAR REMOTE Screen</t>
-        </is>
-      </c>
-      <c r="K13" s="53" t="n"/>
-      <c r="L13" s="54" t="n"/>
-      <c r="M13" s="107" t="n"/>
-      <c r="N13" s="108" t="n"/>
-    </row>
-    <row r="14" ht="160.5" customHeight="1">
-      <c r="B14" s="50" t="n">
-        <v>10</v>
-      </c>
-      <c r="C14" s="51" t="inlineStr">
-        <is>
           <t>EUR, 
 NAR,
 CHN</t>
         </is>
       </c>
-      <c r="D14" s="51" t="inlineStr">
+      <c r="D13" s="51" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E14" s="52" t="n">
+      <c r="E13" s="52" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="190" t="inlineStr">
+      <c r="F13" s="190" t="inlineStr">
         <is>
           <t>Verifying the unit type in My Car Statistics screen by changing unit under Units screen of My Bentley App</t>
         </is>
       </c>
-      <c r="G14" s="190" t="inlineStr">
+      <c r="G13" s="190" t="inlineStr">
         <is>
           <t>The focus of the screen is on Units page. 
 (Login My Bentley App -- &gt;User Profile icon --&gt; Gear icon--&gt; Units)</t>
         </is>
       </c>
-      <c r="H14" s="53" t="n"/>
-      <c r="I14" s="190" t="inlineStr">
+      <c r="H13" s="53" t="n"/>
+      <c r="I13" s="190" t="inlineStr">
         <is>
           <t>1. Change the  metrics / imperial units in 'Units' screen for the below sections : 
 a. UNITS
@@ -13780,17 +13724,18 @@
 2. Observe in MY CAR STATISTICS graphs in ( Car Remote  -- &gt; MY CAR STATISTICS screen )</t>
         </is>
       </c>
-      <c r="J14" s="53" t="inlineStr">
+      <c r="J13" s="53" t="inlineStr">
         <is>
           <t>1. User should be able to change to metrics / imperial units successfully
 2. The selected metrics / imperial units should be visible in Graphical &amp; List view in MY CAR STATISTICS screen</t>
         </is>
       </c>
-      <c r="K14" s="191" t="n"/>
-      <c r="L14" s="54" t="n"/>
-      <c r="M14" s="192" t="n"/>
-      <c r="N14" s="134" t="n"/>
-    </row>
+      <c r="K13" s="191" t="n"/>
+      <c r="L13" s="54" t="n"/>
+      <c r="M13" s="192" t="n"/>
+      <c r="N13" s="134" t="n"/>
+    </row>
+    <row r="14" ht="160.5" customHeight="1"/>
     <row r="15" ht="157.5" customHeight="1"/>
     <row r="16" ht="126" customFormat="1" customHeight="1" s="42">
       <c r="B16" s="12" t="n"/>
@@ -13822,7 +13767,7 @@
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:C3"/>
   </mergeCells>
-  <conditionalFormatting sqref="K5:K14">
+  <conditionalFormatting sqref="K5:K13">
     <cfRule type="cellIs" priority="8" operator="equal" dxfId="13">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -13842,17 +13787,12 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5:L14">
+  <conditionalFormatting sqref="K5:L13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="0">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:L13">
-    <cfRule type="cellIs" priority="52" operator="equal" dxfId="1">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L5:L14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="6">
       <formula>"Cancelled"</formula>
     </cfRule>
@@ -13868,28 +13808,12 @@
     <cfRule type="cellIs" priority="5" operator="equal" dxfId="2">
       <formula>"Blocked"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" priority="43" operator="equal" dxfId="10">
-      <formula>"Not Tested"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="44" operator="equal" dxfId="9">
-      <formula>"Not Applicable"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="45" operator="equal" dxfId="248">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
     <cfRule type="cellIs" priority="6" operator="equal" dxfId="1">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation sqref="K13" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" type="list">
-      <formula1>"Pass,Fail,Not Applicable,Not Tested"</formula1>
-    </dataValidation>
-    <dataValidation sqref="L5:L14" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" type="list">
+  <dataValidations count="1">
+    <dataValidation sqref="L5:L13" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" type="list">
       <formula1>"Pass, Fail, Blocked, NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13953,34 +13877,34 @@
     </row>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="n"/>
-      <c r="B2" s="231" t="inlineStr">
+      <c r="B2" s="241" t="inlineStr">
         <is>
           <t>My Cabin Comfort</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="232" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="242" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="2" t="n"/>
-      <c r="B3" s="233" t="inlineStr">
+      <c r="B3" s="243" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="225" t="n"/>
-      <c r="D3" s="233" t="n"/>
+      <c r="C3" s="235" t="n"/>
+      <c r="D3" s="243" t="n"/>
       <c r="E3" s="48" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t xml:space="preserve">Ensure that below preconditions are met before starting the testing of this service
 • This service applicable for only on PHEV models
@@ -13999,13 +13923,13 @@
 • Make sure that 'My cabin comfort' is not active </t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" s="2" t="inlineStr"/>
@@ -15690,39 +15614,39 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" min="13" max="13"/>
     <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="2" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="2" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="239" t="inlineStr">
+      <c r="B2" s="249" t="inlineStr">
         <is>
           <t>My Battery Charge</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="232" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="242" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="240" t="inlineStr">
+      <c r="B3" s="250" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="31" t="n"/>
       <c r="E3" s="33" t="n"/>
-      <c r="F3" s="238" t="inlineStr">
+      <c r="F3" s="248" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • This service applicable for only on PHEV models
@@ -15734,13 +15658,13 @@
 • Battery Charger connected to Mains Voltage</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="16.5" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -16577,8 +16501,8 @@
   </sheetPr>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
@@ -16597,39 +16521,39 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="16.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="2" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="2" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Service Management</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -16641,13 +16565,13 @@
 • Login to My Bentley App with valid credentials</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -17527,33 +17451,33 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Activate Heating</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Pre Condition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • This service applicable for EU Non-PHEV models
@@ -17565,13 +17489,13 @@
 • Make sure at least 30% of Fuel to be present in Fuel Tank</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -18130,39 +18054,39 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="20.42578125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="2" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="2" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="241" t="inlineStr">
+      <c r="B2" s="251" t="inlineStr">
         <is>
           <t>Roadside Assistance</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="240" t="inlineStr">
+      <c r="B3" s="250" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="31" t="n"/>
       <c r="E3" s="33" t="n"/>
-      <c r="F3" s="238" t="inlineStr">
+      <c r="F3" s="248" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Primary registration process is successfully completed. 
@@ -18171,13 +18095,13 @@
 • Mobile in good network reception area</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="16.5" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -18501,39 +18425,39 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="16.5703125" customWidth="1" style="43" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="43" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="43" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="43" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="43" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Data Services</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -18541,13 +18465,13 @@
 • Login to My Bentley App with valid credentials</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -18980,39 +18904,39 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="15.140625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="2" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="2" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>My Alerts</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="243" t="inlineStr">
+      <c r="B3" s="253" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="227" t="n"/>
+      <c r="C3" s="237" t="n"/>
       <c r="D3" s="178" t="n"/>
       <c r="E3" s="179" t="n"/>
-      <c r="F3" s="242" t="inlineStr">
+      <c r="F3" s="252" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -19021,13 +18945,13 @@
 • Login to My Bentley App with valid credentials</t>
         </is>
       </c>
-      <c r="G3" s="227" t="n"/>
-      <c r="H3" s="227" t="n"/>
-      <c r="I3" s="227" t="n"/>
-      <c r="J3" s="227" t="n"/>
-      <c r="K3" s="227" t="n"/>
-      <c r="L3" s="227" t="n"/>
-      <c r="M3" s="232" t="n"/>
+      <c r="G3" s="237" t="n"/>
+      <c r="H3" s="237" t="n"/>
+      <c r="I3" s="237" t="n"/>
+      <c r="J3" s="237" t="n"/>
+      <c r="K3" s="237" t="n"/>
+      <c r="L3" s="237" t="n"/>
+      <c r="M3" s="242" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -20065,33 +19989,33 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Theft Alarm</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Pre Condition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Theft Alert service is having a valid license and in use
@@ -20101,13 +20025,13 @@
 2. My Bentley mobile app -- &gt; Service Management -- &gt; 'Theft alert' should be enabled</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -20772,28 +20696,28 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="18.7109375" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="46" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="46" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Customer Enrollment</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="30.75" customHeight="1" thickBot="1">
       <c r="B3" s="98" t="inlineStr">
@@ -20804,7 +20728,7 @@
       <c r="C3" s="99" t="n"/>
       <c r="D3" s="100" t="n"/>
       <c r="E3" s="100" t="n"/>
-      <c r="F3" s="230" t="inlineStr">
+      <c r="F3" s="240" t="inlineStr">
         <is>
           <t xml:space="preserve">Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -20816,13 +20740,13 @@
                        3. Set 'Login Method' = 'idk(IDK - Solution)' / 'ping(PING - Solution)'  </t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="30.75" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -23599,33 +23523,33 @@
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Stolen Vehicle Locator</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -23634,13 +23558,13 @@
 • 'Stolen Vehicle Locator' license is valid and in use</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -23976,33 +23900,33 @@
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Audials</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -24010,13 +23934,13 @@
 • Login to My Bentley App with valid credentials</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -24287,33 +24211,33 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Car Finder</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Pre Condition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Car Finder service is having a valid license and in use
@@ -24324,13 +24248,13 @@
  The vehicle is in stationary &amp; connected to the network.</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -24850,39 +24774,39 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="15.42578125" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="2" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="2" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="241" t="inlineStr">
+      <c r="B2" s="251" t="inlineStr">
         <is>
           <t>Nav Companion</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="240" t="inlineStr">
+      <c r="B3" s="250" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="31" t="n"/>
       <c r="E3" s="33" t="n"/>
-      <c r="F3" s="238" t="inlineStr">
+      <c r="F3" s="248" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -24892,13 +24816,13 @@
 • Login to My Bentley App with valid credentials</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -25739,10 +25663,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView topLeftCell="F9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
@@ -25764,33 +25688,33 @@
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Notifications</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -25799,13 +25723,13 @@
 • “My Bentley in Car Services' and 'My Bentley Remote Services' license is valid and in use</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -25966,13 +25890,13 @@
       <c r="M6" s="53" t="n"/>
       <c r="N6" s="55" t="n"/>
     </row>
-    <row r="7" ht="120" customHeight="1">
+    <row r="7" ht="112.5" customHeight="1">
       <c r="B7" s="50" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="51" t="inlineStr">
         <is>
-          <t>EUR , NAR , CHN</t>
+          <t>NAR</t>
         </is>
       </c>
       <c r="D7" s="51" t="inlineStr">
@@ -25981,11 +25905,11 @@
         </is>
       </c>
       <c r="E7" s="52" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="79" t="inlineStr">
         <is>
-          <t>Verify accessing  'Actions' tab in  'Notifications'  screen</t>
+          <t>Verify accessing  'Alert' tab in  'Notifications'  screen</t>
         </is>
       </c>
       <c r="G7" s="53" t="inlineStr">
@@ -25997,14 +25921,14 @@
       <c r="H7" s="53" t="n"/>
       <c r="I7" s="16" t="inlineStr">
         <is>
-          <t>Tap on 'Actions' tab in 'NOTIFICATIONS' page</t>
+          <t>1. Tap on 'Alerts' tab in 'My Bentley App - NOTIFICATIONS' page</t>
         </is>
       </c>
       <c r="J7" s="16" t="inlineStr">
         <is>
-          <t>When there are no actions at all  -&gt;  'There are no new notifications to display' message should be displayed  along with crossed out bell icon 
+          <t>When there are no alerts at all  --&gt;  'There are no new notifications to display' message should be displayed along with crossed out bell icon 
 OTHERWISE
-Maximum 10 actions should be displayed which are sorted by time stamp from newest to oldest.</t>
+Maximum 10 alerts should be displayed which are sorted by time stamp from newest to oldest.</t>
         </is>
       </c>
       <c r="K7" s="53" t="n"/>
@@ -26012,13 +25936,13 @@
       <c r="M7" s="53" t="n"/>
       <c r="N7" s="55" t="n"/>
     </row>
-    <row r="8" ht="135" customHeight="1">
+    <row r="8" ht="174.75" customHeight="1">
       <c r="B8" s="50" t="n">
         <v>4</v>
       </c>
       <c r="C8" s="51" t="inlineStr">
         <is>
-          <t>EUR , NAR , CHN</t>
+          <t>NAR</t>
         </is>
       </c>
       <c r="D8" s="51" t="inlineStr">
@@ -26027,11 +25951,11 @@
         </is>
       </c>
       <c r="E8" s="52" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F8" s="79" t="inlineStr">
         <is>
-          <t>Verify the contents of an action in 'Actions' tab in Notification Screen</t>
+          <t>Verify 'Alerts' are listed in the notification Alert list</t>
         </is>
       </c>
       <c r="G8" s="53" t="inlineStr">
@@ -26042,20 +25966,20 @@
       </c>
       <c r="H8" s="53" t="inlineStr">
         <is>
-          <t>• At least one Action should be present  in the 'Actions' list (e.g. Perform Remote Lock / Unlock operation through App)</t>
-        </is>
-      </c>
-      <c r="I8" s="16" t="inlineStr">
-        <is>
-          <t>Tap on 'Actions' tab in 'NOTIFICATIONS' page and check the contents of any listed action</t>
-        </is>
-      </c>
-      <c r="J8" s="16" t="inlineStr">
-        <is>
-          <t>Each action should have following contents in sequence
-- Status on the actions (e.g. 'Vehicle Locked/Unlocked/Failed to Lock/Failed to unlock' etc.)
-- Time stamp(e.g. 24 January 09.37 am)
-- Summary/Reasons (e.g. Vehicle was successfully locked/unlocked or Failed Reason)</t>
+          <t>1. Perform multiple 'Alert'( Ex : Speed Alert, Curfew Alert , Valet Alert  and Perimeter Alert ) functionality in different scenario</t>
+        </is>
+      </c>
+      <c r="I8" s="53" t="inlineStr">
+        <is>
+          <t>1. Refresh the 'NOTIFICATIONS - Alertss' page and Check whether all alerts related to 'Speed , Curfew , Valet &amp; Perimeter - Alerts' listed under 'My Bentley App - NAVIGATIONS - Alerts' screen</t>
+        </is>
+      </c>
+      <c r="J8" s="53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1. Multiple Alert( Ex : Speed Alert, Curfew Alert , Valet Alert  and Perimeter Alert ) functionality scenarios are performed successfully without any issues
+2. All Alerts related to 'Speed , Curfew , Valet &amp; Perimeter - Alerts' should be listed in under 'My Bentley App - NAVIGATIONS - Alerts' screen and sorted by time stamp from newest to oldest.
+[Ex :1. On event occurs -&gt; Status : xxxxxxxx,  Time Stamp : 'DD Month hh.ss am/pm', Summary: 'xxxxxx']
+</t>
         </is>
       </c>
       <c r="K8" s="53" t="n"/>
@@ -26063,202 +25987,59 @@
       <c r="M8" s="53" t="n"/>
       <c r="N8" s="55" t="n"/>
     </row>
-    <row r="9" ht="393.75" customHeight="1">
-      <c r="B9" s="50" t="n">
+    <row r="9" ht="47.25" customHeight="1" thickBot="1">
+      <c r="B9" s="59" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="51" t="inlineStr">
+      <c r="C9" s="60" t="inlineStr">
         <is>
           <t>EUR , NAR , CHN</t>
         </is>
       </c>
-      <c r="D9" s="51" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="E9" s="52" t="n">
+      <c r="D9" s="60" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E9" s="61" t="n">
         <v>10</v>
       </c>
-      <c r="F9" s="79" t="inlineStr">
-        <is>
-          <t>Verify 'Remote Lock / Unlock' actions are listed in the notification action list</t>
-        </is>
-      </c>
-      <c r="G9" s="53" t="inlineStr">
-        <is>
-          <t>• The screen focus is in "My Bentley App - NOTIFICATIONS" page
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; Click on "Bell" icon (NOTIFICATIONS) )</t>
+      <c r="F9" s="94" t="inlineStr">
+        <is>
+          <t>Verify all the screen with Bentley style guide.</t>
+        </is>
+      </c>
+      <c r="G9" s="62" t="inlineStr">
+        <is>
+          <t>• N/A</t>
         </is>
       </c>
       <c r="H9" s="53" t="n"/>
-      <c r="I9" s="53" t="inlineStr">
-        <is>
-          <t>1. Perform multiple 'Remote Lock / Unlock' functionality in different scenarios (E.g. Ignition On, Off) through 'My Bentley App - DASHBOARD' screen
-2. Refresh the 'NOTIFICATIONS - Actions' page and Check whether 'Remote Lock / Unlock' functionality actions are listed</t>
-        </is>
-      </c>
-      <c r="J9" s="53" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1. 'Remote Lock / Unlock' functionality in different scenarios (E.g. Ignition On, Off) are successfully performed through 'My Bentley App - DASHBOARD' screen
-2. All performed actions related to 'Remote Lock / Unlock' functionality should be listed in under 'My Bentley App - NAVIGATIONS - Actions' screen and sorted by time stamp from newest to oldest.
-[Ex :  1. On Successful Lock/Unlock Actions --&gt; Status : 'XX (Vehicle Name) Locked/Unlocked' , Time Stamp : 'DD Month hh.ss am/pm', Summary: 'XX successfully locked/unlocked']
-[Ex :  2. On Failure to Lock/Unlock Actions -&gt; Status: 'Failed to unlock XX(Vehicle Name)', Time Stamp : 'DD Month hh.ss am/pm', Reason: 'Please Close the Driver door' Or 'Battery Drain State -Unable to reach the vehicle' etc.] 
-</t>
-        </is>
-      </c>
-      <c r="K9" s="53" t="n"/>
-      <c r="L9" s="54" t="n"/>
-      <c r="M9" s="53" t="n"/>
-      <c r="N9" s="55" t="n"/>
-    </row>
-    <row r="10" ht="120" customHeight="1">
-      <c r="B10" s="50" t="n">
-        <v>6</v>
-      </c>
-      <c r="C10" s="51" t="inlineStr">
-        <is>
-          <t>NAR</t>
-        </is>
-      </c>
-      <c r="D10" s="51" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="E10" s="52" t="n">
-        <v>3</v>
-      </c>
-      <c r="F10" s="79" t="inlineStr">
-        <is>
-          <t>Verify accessing  'Alert' tab in  'Notifications'  screen</t>
-        </is>
-      </c>
-      <c r="G10" s="53" t="inlineStr">
-        <is>
-          <t>• The screen focus is in "My Bentley App - NOTIFICATIONS" page
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; Click on "Bell" icon (NOTIFICATIONS) )</t>
-        </is>
-      </c>
-      <c r="H10" s="53" t="n"/>
-      <c r="I10" s="16" t="inlineStr">
-        <is>
-          <t>1. Tap on 'Alerts' tab in 'My Bentley App - NOTIFICATIONS' page</t>
-        </is>
-      </c>
-      <c r="J10" s="16" t="inlineStr">
-        <is>
-          <t>When there are no alerts at all  --&gt;  'There are no new notifications to display' message should be displayed along with crossed out bell icon 
-OTHERWISE
-Maximum 10 alerts should be displayed which are sorted by time stamp from newest to oldest.</t>
-        </is>
-      </c>
-      <c r="K10" s="53" t="n"/>
-      <c r="L10" s="54" t="n"/>
-      <c r="M10" s="53" t="n"/>
-      <c r="N10" s="55" t="n"/>
-    </row>
-    <row r="11" ht="252" customHeight="1">
-      <c r="B11" s="50" t="n">
-        <v>7</v>
-      </c>
-      <c r="C11" s="51" t="inlineStr">
-        <is>
-          <t>NAR</t>
-        </is>
-      </c>
-      <c r="D11" s="51" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="E11" s="52" t="n">
-        <v>15</v>
-      </c>
-      <c r="F11" s="79" t="inlineStr">
-        <is>
-          <t>Verify 'Alerts' are listed in the notification Alert list</t>
-        </is>
-      </c>
-      <c r="G11" s="53" t="inlineStr">
-        <is>
-          <t>• The screen focus is in "My Bentley App - NOTIFICATIONS" page
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen --&gt; Click on "Bell" icon (NOTIFICATIONS) )</t>
-        </is>
-      </c>
-      <c r="H11" s="53" t="inlineStr">
-        <is>
-          <t>1. Perform multiple 'Alert'( Ex : Speed Alert, Curfew Alert , Valet Alert  and Perimeter Alert ) functionality in different scenario</t>
-        </is>
-      </c>
-      <c r="I11" s="53" t="inlineStr">
-        <is>
-          <t>1. Refresh the 'NOTIFICATIONS - Alertss' page and Check whether all alerts related to 'Speed , Curfew , Valet &amp; Perimeter - Alerts' listed under 'My Bentley App - NAVIGATIONS - Alerts' screen</t>
-        </is>
-      </c>
-      <c r="J11" s="53" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1. Multiple Alert( Ex : Speed Alert, Curfew Alert , Valet Alert  and Perimeter Alert ) functionality scenarios are performed successfully without any issues
-2. All Alerts related to 'Speed , Curfew , Valet &amp; Perimeter - Alerts' should be listed in under 'My Bentley App - NAVIGATIONS - Alerts' screen and sorted by time stamp from newest to oldest.
-[Ex :1. On event occurs -&gt; Status : xxxxxxxx,  Time Stamp : 'DD Month hh.ss am/pm', Summary: 'xxxxxx']
-</t>
-        </is>
-      </c>
-      <c r="K11" s="53" t="n"/>
-      <c r="L11" s="54" t="n"/>
-      <c r="M11" s="53" t="n"/>
-      <c r="N11" s="55" t="n"/>
-    </row>
-    <row r="12" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B12" s="59" t="n">
-        <v>8</v>
-      </c>
-      <c r="C12" s="60" t="inlineStr">
-        <is>
-          <t>EUR , NAR , CHN</t>
-        </is>
-      </c>
-      <c r="D12" s="60" t="inlineStr">
-        <is>
-          <t>Low</t>
-        </is>
-      </c>
-      <c r="E12" s="61" t="n">
-        <v>10</v>
-      </c>
-      <c r="F12" s="94" t="inlineStr">
-        <is>
-          <t>Verify all the screen with Bentley style guide.</t>
-        </is>
-      </c>
-      <c r="G12" s="62" t="inlineStr">
-        <is>
-          <t>• N/A</t>
-        </is>
-      </c>
-      <c r="H12" s="53" t="n"/>
-      <c r="I12" s="62" t="inlineStr">
+      <c r="I9" s="62" t="inlineStr">
         <is>
           <t>Observe all the screen's icon, font, colour</t>
         </is>
       </c>
-      <c r="J12" s="62" t="inlineStr">
+      <c r="J9" s="62" t="inlineStr">
         <is>
           <t>All the icon, font, colour should be followed as per Bentley style guide.</t>
         </is>
       </c>
-      <c r="K12" s="62" t="n"/>
-      <c r="L12" s="63" t="n"/>
-      <c r="M12" s="62" t="n"/>
-      <c r="N12" s="64" t="n"/>
-    </row>
+      <c r="K9" s="62" t="n"/>
+      <c r="L9" s="63" t="n"/>
+      <c r="M9" s="62" t="n"/>
+      <c r="N9" s="64" t="n"/>
+    </row>
+    <row r="10" ht="120" customHeight="1"/>
+    <row r="11" ht="252" customHeight="1"/>
+    <row r="12" ht="32.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="F3:M3"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:C3"/>
   </mergeCells>
-  <conditionalFormatting sqref="K5:K11">
+  <conditionalFormatting sqref="K5:K8">
     <cfRule type="cellIs" priority="8" operator="equal" dxfId="13">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -26281,7 +26062,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5:L12">
+  <conditionalFormatting sqref="L5:L9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="6">
       <formula>"Cancelled"</formula>
     </cfRule>
@@ -26305,7 +26086,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation sqref="L5:L12" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" type="list">
+    <dataValidation sqref="L5:L9" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" type="list">
       <formula1>"Pass, Fail, Blocked, NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -26354,33 +26135,33 @@
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Push Notifications</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -26389,13 +26170,13 @@
 • “My Bentley in Car Services' and 'My Bentley Remote Services' license is valid and in use</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -27078,46 +26859,46 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Profile</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Pre Condition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Primary user successfully  registered with vehicle
 • My Bentley mobile app should have valid credentials.</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -28280,39 +28061,39 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="14" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="46" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="46" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Localization</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -28322,13 +28103,13 @@
 • Login to My Bentley App with valid credentials</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -28596,33 +28377,33 @@
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="241" t="inlineStr">
+      <c r="B2" s="251" t="inlineStr">
         <is>
           <t>Privacy Mode</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="240" t="inlineStr">
+      <c r="B3" s="250" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="31" t="n"/>
       <c r="E3" s="33" t="n"/>
-      <c r="F3" s="238" t="inlineStr">
+      <c r="F3" s="248" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -28630,13 +28411,13 @@
 • “My Bentley in Car Services' and 'My Bentley Remote Services' license is valid and in use</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" t="inlineStr"/>
@@ -29663,33 +29444,33 @@
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Remote Park Assist</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -29700,13 +29481,13 @@
 • Test Mobile where My Bentley App is installed is paired to Head Unit via Bluetooth</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -33280,8 +33061,8 @@
   </sheetPr>
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
@@ -33303,33 +33084,33 @@
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Add VIN</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t xml:space="preserve">Ensure that below preconditions are met before start the testing for this service
 • My Bentley in Car Services' and 'My Bentley Remote Services' license is valid and in use
@@ -33343,13 +33124,13 @@
                        3. Set 'Login Method' = 'idk(IDK - Solution)' / 'ping(PING - Solution)'   </t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -33722,29 +33503,29 @@
       <c r="N10" s="88" t="n"/>
     </row>
     <row r="11" ht="169.5" customHeight="1">
-      <c r="B11" s="82" t="n">
+      <c r="B11" s="223" t="n">
         <v>7</v>
       </c>
-      <c r="C11" s="83" t="inlineStr">
+      <c r="C11" s="224" t="inlineStr">
         <is>
           <t>EUR, NAR, CHN</t>
         </is>
       </c>
-      <c r="D11" s="83" t="inlineStr">
+      <c r="D11" s="224" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E11" s="84">
+      <c r="E11" s="225">
         <f>(5+3+3)/3</f>
         <v/>
       </c>
-      <c r="F11" s="79" t="inlineStr">
+      <c r="F11" s="226" t="inlineStr">
         <is>
           <t>Verify validating camera when 'Open Camera' Link option selected from ADD A VEHICLE screen in My Bentley App</t>
         </is>
       </c>
-      <c r="G11" s="111" t="inlineStr">
+      <c r="G11" s="227" t="inlineStr">
         <is>
           <t>• Login to My Bentley App with valid credentials
 • The screen focus is in "My Bentley App - ADD A VEHICLE" page
@@ -33752,15 +33533,15 @@
 • Permission to access camera is already given to My Bentley App</t>
         </is>
       </c>
-      <c r="H11" s="111" t="n"/>
-      <c r="I11" s="128" t="inlineStr">
+      <c r="H11" s="227" t="n"/>
+      <c r="I11" s="228" t="inlineStr">
         <is>
           <t xml:space="preserve">Validate  'ADD A VEHICLE' Screen : 
 1. In 'ADD A VEHICLE' screen, Click on 'Open Camera' Link and observe
 </t>
         </is>
       </c>
-      <c r="J11" s="130" t="inlineStr">
+      <c r="J11" s="229" t="inlineStr">
         <is>
           <t xml:space="preserve">1. Clicking on 'Open Camera' Link in 'ADD A VEHICLE' screen should launch camera displaying
 a. Virtual Box to centre the VIN for capturing via camera
@@ -33768,12 +33549,12 @@
 c. Flash button </t>
         </is>
       </c>
-      <c r="K11" s="79" t="n"/>
-      <c r="L11" s="86" t="n"/>
-      <c r="M11" s="87" t="n"/>
-      <c r="N11" s="88" t="n"/>
-    </row>
-    <row r="12" ht="168" customHeight="1">
+      <c r="K11" s="226" t="n"/>
+      <c r="L11" s="230" t="n"/>
+      <c r="M11" s="231" t="n"/>
+      <c r="N11" s="232" t="n"/>
+    </row>
+    <row r="12" ht="188.45" customHeight="1">
       <c r="B12" s="82" t="n">
         <v>8</v>
       </c>
@@ -33793,7 +33574,7 @@
       </c>
       <c r="F12" s="79" t="inlineStr">
         <is>
-          <t>Verify capturing VIN when via Camera [ Flash = Off ]</t>
+          <t>Verify capturing VIN when via Camera [ Flash = Off ] and validate 'Scan VIN again' option under 'ADD A VEHICLE - CONFIRM YOUR VIN' Screen</t>
         </is>
       </c>
       <c r="G12" s="111" t="inlineStr">
@@ -33811,14 +33592,17 @@
 1. In 'ADD A VEHICLE' screen, Click on 'Open Camera' Link
 2. Flash = Off
 3. Centre focus the VIN in the virtual box in Camera and capture the photo
-</t>
+4. Click on 'Scan VIN again' option and Observe
+My Bentley App : 
+( ADD A VEHICLE screen --&gt; Click on 'ADD A VEHICLE' button --&gt; Open Camera  --&gt; Mobile Camera should be launched --&gt; Centre your VIN in the box specified in camera for capturing VIN --&gt; Capture VIN Photo --&gt; VIN added to 'ADD A VEHICLE - CONFIRM YOUR VIN' screen  --&gt; Click on 'Scan VIN again' ) </t>
         </is>
       </c>
       <c r="J12" s="130" t="inlineStr">
         <is>
           <t>1. Clicking on 'Open Camera' Link in 'ADD A VEHICLE' screen should launch camera
 2. Flash is not enabled
-3. VIN should be successfully captured without flash via camera and should be successfully added to VIN field</t>
+3. VIN should be successfully captured without flash via camera and should be successfully added to VIN field
+4. The Mobile Camera should be relaunched when user clicks on 'Scan VIN again'</t>
         </is>
       </c>
       <c r="K12" s="79" t="n"/>
@@ -34084,29 +33868,29 @@
       <c r="N17" s="88" t="n"/>
     </row>
     <row r="18" ht="195" customHeight="1">
-      <c r="B18" s="82" t="n">
+      <c r="B18" s="223" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="83" t="inlineStr">
+      <c r="C18" s="224" t="inlineStr">
         <is>
           <t>EUR, NAR, CHN</t>
         </is>
       </c>
-      <c r="D18" s="83" t="inlineStr">
+      <c r="D18" s="224" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="E18" s="84">
+      <c r="E18" s="225">
         <f>(3+2+3)/3</f>
         <v/>
       </c>
-      <c r="F18" s="79" t="inlineStr">
+      <c r="F18" s="226" t="inlineStr">
         <is>
           <t>Verify validating 'Scan VIN again' option under 'ADD A VEHICLE - CONFIRM YOUR VIN' Screen</t>
         </is>
       </c>
-      <c r="G18" s="111" t="inlineStr">
+      <c r="G18" s="227" t="inlineStr">
         <is>
           <t>• Login to My Bentley App with valid credentials
 • The screen focus is in "My Bentley App - ADD A VEHICLE" page
@@ -34114,8 +33898,8 @@
 • Permission to access camera is already given to My Bentley App</t>
         </is>
       </c>
-      <c r="H18" s="111" t="n"/>
-      <c r="I18" s="128" t="inlineStr">
+      <c r="H18" s="227" t="n"/>
+      <c r="I18" s="228" t="inlineStr">
         <is>
           <t xml:space="preserve">Add VIN - Optical Character Recognition(OCR) -  'ADD A VEHICLE' Screen - Camera Permission - Given :
 1. In 'ADD A VEHICLE -  CONFIRM YOUR VIN' screen  --&gt; Click on 'Scan VIN again' option and Observe
@@ -34124,15 +33908,15 @@
 </t>
         </is>
       </c>
-      <c r="J18" s="130" t="inlineStr">
+      <c r="J18" s="229" t="inlineStr">
         <is>
           <t xml:space="preserve">1. The Mobile Camera should be relaunched displaying a box stating Msg(Centre your VIN in the box above) when user clicks on 'Scan VIN again' option under 'ADD A VEHICLE - CONFIRM YOUR VIN' screen </t>
         </is>
       </c>
-      <c r="K18" s="79" t="n"/>
-      <c r="L18" s="86" t="n"/>
-      <c r="M18" s="87" t="n"/>
-      <c r="N18" s="88" t="n"/>
+      <c r="K18" s="226" t="n"/>
+      <c r="L18" s="230" t="n"/>
+      <c r="M18" s="231" t="n"/>
+      <c r="N18" s="232" t="n"/>
     </row>
     <row r="19" ht="165" customHeight="1">
       <c r="B19" s="82" t="n">
@@ -34358,7 +34142,7 @@
   </sheetPr>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D29" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
@@ -34381,33 +34165,33 @@
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Stolen Vehicle Tracking</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>1. Before starting each scenario, Please follow : 
 a. Ignition = Off
@@ -34416,13 +34200,13 @@
 d. While performing drive scenarios, Request to drive for &gt;500 m with Speed &gt;8Km/Hr on a straight road</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -38701,39 +38485,39 @@
     <col width="19.42578125" customWidth="1" style="43" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="43" min="13" max="13"/>
     <col width="15.5703125" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="46" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="46" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>App Registration Pages</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t xml:space="preserve">Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -38745,13 +38529,13 @@
                        3. Set 'Login Method' = 'idk(IDK - Solution)' / 'ping(PING - Solution)'  </t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1">
       <c r="A4" t="inlineStr"/>
@@ -39367,46 +39151,46 @@
     </row>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="n"/>
-      <c r="B2" s="231" t="inlineStr">
+      <c r="B2" s="241" t="inlineStr">
         <is>
           <t>App Log in-Log out</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="232" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="242" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="2" t="n"/>
-      <c r="B3" s="233" t="inlineStr">
+      <c r="B3" s="243" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="225" t="n"/>
-      <c r="D3" s="233" t="n"/>
+      <c r="C3" s="235" t="n"/>
+      <c r="D3" s="243" t="n"/>
       <c r="E3" s="48" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before starting the testing of this service
 • My Bentley app should be installed in the mobile</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="32.25" customHeight="1" thickBot="1">
       <c r="A4" s="2" t="inlineStr"/>
@@ -39911,8 +39695,8 @@
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -39931,8 +39715,8 @@
     <col width="19.42578125" customWidth="1" style="46" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="46" min="13" max="13"/>
     <col width="14.85546875" customWidth="1" style="46" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="46" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="46" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="46" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="46" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1">
@@ -39952,34 +39736,34 @@
     </row>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
       <c r="A2" s="43" t="n"/>
-      <c r="B2" s="231" t="inlineStr">
+      <c r="B2" s="241" t="inlineStr">
         <is>
           <t>Nickname</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="232" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="242" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="43" t="n"/>
-      <c r="B3" s="233" t="inlineStr">
+      <c r="B3" s="243" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="225" t="n"/>
-      <c r="D3" s="233" t="n"/>
+      <c r="C3" s="235" t="n"/>
+      <c r="D3" s="243" t="n"/>
       <c r="E3" s="48" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before starting the testing of this service
 • My Bentley app should be installed in the mobile
@@ -39987,13 +39771,13 @@
 • Primary user registration process is completed successfully</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" s="43" t="inlineStr"/>
@@ -40178,15 +39962,12 @@
       </c>
       <c r="G7" s="53" t="inlineStr">
         <is>
-          <t>• The screen focus is in "My Bentley App - DASHBOARD" page
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen )</t>
-        </is>
-      </c>
-      <c r="H7" s="53" t="inlineStr">
-        <is>
-          <t xml:space="preserve">• Nickname to vehicle is not added </t>
-        </is>
-      </c>
+          <t xml:space="preserve">• The screen focus is in "My Bentley App - DASHBOARD" page
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen )
+• Nickname to vehicle is not added </t>
+        </is>
+      </c>
+      <c r="H7" s="53" t="n"/>
       <c r="I7" s="53" t="inlineStr">
         <is>
           <t>1. In vehicle 'DASHBOARD' screen, Click on 'i-icon' present at top right corner of screen
@@ -40288,15 +40069,12 @@
       </c>
       <c r="G9" s="53" t="inlineStr">
         <is>
-          <t>• The screen focus is in "My Bentley App - DASHBOARD" page
-( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen )</t>
-        </is>
-      </c>
-      <c r="H9" s="53" t="inlineStr">
-        <is>
-          <t xml:space="preserve">• Nickname to vehicle already added </t>
-        </is>
-      </c>
+          <t xml:space="preserve">• The screen focus is in "My Bentley App - DASHBOARD" page
+( My Bentley App --&gt; LOGIN OR REGISTER --&gt; Email --&gt; Enter valid email id --&gt; NEXT --&gt; Enter the Password --&gt; NEXT --&gt; Vehicle "DASHBOARD" Screen )
+• Nickname to vehicle is added </t>
+        </is>
+      </c>
+      <c r="H9" s="53" t="n"/>
       <c r="I9" s="53" t="inlineStr">
         <is>
           <t>1. In vehicle 'DASHBOARD' screen, Click on 'i-icon' present at top right corner of screen
@@ -40688,41 +40466,41 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="15.85546875" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="2" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="2" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
       <c r="A2" s="43" t="n"/>
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Services and licenses</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="43" t="n"/>
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -40732,13 +40510,13 @@
 • Login to My Bentley App with valid credentials</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" s="43" t="inlineStr"/>
@@ -41485,8 +41263,8 @@
   </sheetPr>
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.7109375" defaultRowHeight="15.75"/>
@@ -41505,52 +41283,52 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="14.7109375" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="2" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="2" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="226" t="inlineStr">
+      <c r="B2" s="236" t="inlineStr">
         <is>
           <t>Vehicle Status Report</t>
         </is>
       </c>
-      <c r="C2" s="227" t="n"/>
-      <c r="D2" s="227" t="n"/>
-      <c r="E2" s="227" t="n"/>
-      <c r="F2" s="227" t="n"/>
-      <c r="G2" s="227" t="n"/>
-      <c r="H2" s="227" t="n"/>
-      <c r="I2" s="227" t="n"/>
-      <c r="J2" s="227" t="n"/>
-      <c r="K2" s="227" t="n"/>
-      <c r="L2" s="227" t="n"/>
-      <c r="M2" s="228" t="n"/>
+      <c r="C2" s="237" t="n"/>
+      <c r="D2" s="237" t="n"/>
+      <c r="E2" s="237" t="n"/>
+      <c r="F2" s="237" t="n"/>
+      <c r="G2" s="237" t="n"/>
+      <c r="H2" s="237" t="n"/>
+      <c r="I2" s="237" t="n"/>
+      <c r="J2" s="237" t="n"/>
+      <c r="K2" s="237" t="n"/>
+      <c r="L2" s="237" t="n"/>
+      <c r="M2" s="238" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="229" t="inlineStr">
+      <c r="B3" s="239" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="224" t="n"/>
+      <c r="C3" s="234" t="n"/>
       <c r="D3" s="68" t="n"/>
       <c r="E3" s="69" t="n"/>
-      <c r="F3" s="223" t="inlineStr">
+      <c r="F3" s="233" t="inlineStr">
         <is>
           <t>Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
 • Primary user registration process is completed successfully</t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="225" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="235" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>
@@ -41642,11 +41420,7 @@
           <t>Access 'Vehicle Status Report(VSR)' service from Mobile App</t>
         </is>
       </c>
-      <c r="G5" s="120" t="inlineStr">
-        <is>
-          <t>• NA</t>
-        </is>
-      </c>
+      <c r="G5" s="120" t="n"/>
       <c r="H5" s="53" t="n"/>
       <c r="I5" s="120" t="inlineStr">
         <is>
@@ -41932,7 +41706,7 @@
     </row>
     <row r="11" ht="150.75" customHeight="1">
       <c r="B11" s="50" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11" s="51" t="inlineStr">
         <is>
@@ -41979,7 +41753,7 @@
     </row>
     <row r="12" ht="135.75" customHeight="1">
       <c r="B12" s="50" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="51" t="inlineStr">
         <is>
@@ -42026,7 +41800,7 @@
     </row>
     <row r="13" ht="145.5" customHeight="1">
       <c r="B13" s="50" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" s="51" t="inlineStr">
         <is>
@@ -42073,7 +41847,7 @@
     </row>
     <row r="14" ht="110.25" customHeight="1">
       <c r="B14" s="50" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" s="51" t="inlineStr">
         <is>
@@ -42125,7 +41899,7 @@
     </row>
     <row r="15" ht="110.25" customHeight="1">
       <c r="B15" s="50" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C15" s="51" t="inlineStr">
         <is>
@@ -43322,39 +43096,39 @@
     <col width="19.42578125" customWidth="1" style="2" min="12" max="12"/>
     <col width="18.85546875" customWidth="1" style="2" min="13" max="13"/>
     <col width="14.140625" customWidth="1" style="2" min="14" max="14"/>
-    <col width="8.7109375" customWidth="1" style="2" min="15" max="52"/>
-    <col width="8.7109375" customWidth="1" style="2" min="53" max="16384"/>
+    <col width="8.7109375" customWidth="1" style="2" min="15" max="60"/>
+    <col width="8.7109375" customWidth="1" style="2" min="61" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1" thickBot="1"/>
     <row r="2" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B2" s="236" t="inlineStr">
+      <c r="B2" s="246" t="inlineStr">
         <is>
           <t>Remote Lock-Unlock</t>
         </is>
       </c>
-      <c r="C2" s="224" t="n"/>
-      <c r="D2" s="224" t="n"/>
-      <c r="E2" s="224" t="n"/>
-      <c r="F2" s="224" t="n"/>
-      <c r="G2" s="224" t="n"/>
-      <c r="H2" s="224" t="n"/>
-      <c r="I2" s="224" t="n"/>
-      <c r="J2" s="224" t="n"/>
-      <c r="K2" s="224" t="n"/>
-      <c r="L2" s="224" t="n"/>
-      <c r="M2" s="235" t="n"/>
+      <c r="C2" s="234" t="n"/>
+      <c r="D2" s="234" t="n"/>
+      <c r="E2" s="234" t="n"/>
+      <c r="F2" s="234" t="n"/>
+      <c r="G2" s="234" t="n"/>
+      <c r="H2" s="234" t="n"/>
+      <c r="I2" s="234" t="n"/>
+      <c r="J2" s="234" t="n"/>
+      <c r="K2" s="234" t="n"/>
+      <c r="L2" s="234" t="n"/>
+      <c r="M2" s="245" t="n"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" thickBot="1">
-      <c r="B3" s="237" t="inlineStr">
+      <c r="B3" s="247" t="inlineStr">
         <is>
           <t>Precondition</t>
         </is>
       </c>
-      <c r="C3" s="235" t="n"/>
+      <c r="C3" s="245" t="n"/>
       <c r="D3" s="187" t="n"/>
       <c r="E3" s="188" t="n"/>
-      <c r="F3" s="234" t="inlineStr">
+      <c r="F3" s="244" t="inlineStr">
         <is>
           <t xml:space="preserve">Ensure that below preconditions are met before start the testing for this service
 • Vehicle is connected to network 
@@ -43365,13 +43139,13 @@
 </t>
         </is>
       </c>
-      <c r="G3" s="224" t="n"/>
-      <c r="H3" s="224" t="n"/>
-      <c r="I3" s="224" t="n"/>
-      <c r="J3" s="224" t="n"/>
-      <c r="K3" s="224" t="n"/>
-      <c r="L3" s="224" t="n"/>
-      <c r="M3" s="235" t="n"/>
+      <c r="G3" s="234" t="n"/>
+      <c r="H3" s="234" t="n"/>
+      <c r="I3" s="234" t="n"/>
+      <c r="J3" s="234" t="n"/>
+      <c r="K3" s="234" t="n"/>
+      <c r="L3" s="234" t="n"/>
+      <c r="M3" s="245" t="n"/>
     </row>
     <row r="4" ht="48" customHeight="1" thickBot="1">
       <c r="A4" t="inlineStr"/>

</xml_diff>